<commit_message>
feat: adicionado ajustes no modelo
</commit_message>
<xml_diff>
--- a/jupyter/notebooks/playground/maycon/modelagem/validacao.xlsx
+++ b/jupyter/notebooks/playground/maycon/modelagem/validacao.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="300">
   <si>
     <t>id</t>
   </si>
@@ -43,84 +43,6 @@
     <t>Positiva</t>
   </si>
   <si>
-    <t>6WANxDZeJW</t>
-  </si>
-  <si>
-    <t>AFcA-c56sW</t>
-  </si>
-  <si>
-    <t>0H-kLj4Zid</t>
-  </si>
-  <si>
-    <t>f-jgDjYRuF</t>
-  </si>
-  <si>
-    <t>DeRljaQILy</t>
-  </si>
-  <si>
-    <t>-CXZ5tBSAg</t>
-  </si>
-  <si>
-    <t>GkOlj1itSF</t>
-  </si>
-  <si>
-    <t>cVLzPxay3y</t>
-  </si>
-  <si>
-    <t>KYmJXL8T0i</t>
-  </si>
-  <si>
-    <t>S14_BOYNcx</t>
-  </si>
-  <si>
-    <t>itrouw6GAb</t>
-  </si>
-  <si>
-    <t>6a-j1VlCrt</t>
-  </si>
-  <si>
-    <t>261r2_b-pa</t>
-  </si>
-  <si>
-    <t>WBEWhctzgb</t>
-  </si>
-  <si>
-    <t>chybTSj7Zh</t>
-  </si>
-  <si>
-    <t>dlTj4Z64vh</t>
-  </si>
-  <si>
-    <t>PsHn2OjzAN</t>
-  </si>
-  <si>
-    <t>1bMi2yPzC4</t>
-  </si>
-  <si>
-    <t>ksRGb9gGig</t>
-  </si>
-  <si>
-    <t>OEaTwBChCy</t>
-  </si>
-  <si>
-    <t>77lLV97i8e</t>
-  </si>
-  <si>
-    <t>O3Lb-tPoEa</t>
-  </si>
-  <si>
-    <t>wtYQC0AL86</t>
-  </si>
-  <si>
-    <t>rASALqlqS3</t>
-  </si>
-  <si>
-    <t>BD5U6n9CG7</t>
-  </si>
-  <si>
-    <t>kbryQop5D3</t>
-  </si>
-  <si>
     <t>fTnYCuIMCz</t>
   </si>
   <si>
@@ -133,33 +55,105 @@
     <t>1NEcEK8DCJ</t>
   </si>
   <si>
+    <t>aV7UyK4RZM</t>
+  </si>
+  <si>
+    <t>xpbpLS477K</t>
+  </si>
+  <si>
+    <t>soE5_SRLGW</t>
+  </si>
+  <si>
     <t>1muufGAMr_</t>
   </si>
   <si>
+    <t>KMFY9vmHJv</t>
+  </si>
+  <si>
+    <t>nFDOOy5VrL</t>
+  </si>
+  <si>
+    <t>LOGA1ClkXg</t>
+  </si>
+  <si>
     <t>JHcB5RLVwN</t>
   </si>
   <si>
     <t>IV7mOWePyt</t>
   </si>
   <si>
+    <t>WuD6rWd4SN</t>
+  </si>
+  <si>
     <t>qVxi-4og0n</t>
   </si>
   <si>
+    <t>PpHudG5gZI</t>
+  </si>
+  <si>
+    <t>JHzJajomkf</t>
+  </si>
+  <si>
+    <t>KwrDPtUxwb</t>
+  </si>
+  <si>
+    <t>QrJ5Fbcyov</t>
+  </si>
+  <si>
+    <t>griwNBkhLh</t>
+  </si>
+  <si>
     <t>TLe3ydgRrq</t>
   </si>
   <si>
     <t>MAz7mWBrbo</t>
   </si>
   <si>
+    <t>1ti-bvq7pa</t>
+  </si>
+  <si>
+    <t>MgXNmqGHVk</t>
+  </si>
+  <si>
+    <t>pYekL2-6VP</t>
+  </si>
+  <si>
+    <t>SiFeQiICA5</t>
+  </si>
+  <si>
+    <t>JhCNbxgBO5</t>
+  </si>
+  <si>
+    <t>P_UrBkViv_</t>
+  </si>
+  <si>
     <t>4Mt8kjbMsf</t>
   </si>
   <si>
+    <t>tSLe4YHcjK</t>
+  </si>
+  <si>
     <t>Mlrz3YmJHI</t>
   </si>
   <si>
+    <t>BAM82rUXIb</t>
+  </si>
+  <si>
+    <t>Kc-FjFleUH</t>
+  </si>
+  <si>
+    <t>y-jPylkXbE</t>
+  </si>
+  <si>
     <t>Ah6rMXdqdr</t>
   </si>
   <si>
+    <t>zsNrxiisid</t>
+  </si>
+  <si>
+    <t>Is2n7pZmY5</t>
+  </si>
+  <si>
     <t>euuDAfLyIb</t>
   </si>
   <si>
@@ -172,85 +166,109 @@
     <t>oXLivTWG_L</t>
   </si>
   <si>
+    <t>c2eTyfZAH8</t>
+  </si>
+  <si>
+    <t>8NTk19dZPa</t>
+  </si>
+  <si>
+    <t>PPzo1oiCTi</t>
+  </si>
+  <si>
+    <t>ZMhiSD6Rk2</t>
+  </si>
+  <si>
+    <t>QUImkcAz6I</t>
+  </si>
+  <si>
     <t>AKysxB8_WN</t>
   </si>
   <si>
+    <t>z5iF43aF1y</t>
+  </si>
+  <si>
+    <t>78dijwUJ8C</t>
+  </si>
+  <si>
+    <t>67nRmTzCS7</t>
+  </si>
+  <si>
+    <t>pnESr5yubn</t>
+  </si>
+  <si>
     <t>WYjLdY0iNB</t>
   </si>
   <si>
+    <t>8UaJUgdVoh</t>
+  </si>
+  <si>
+    <t>IARZDFcVlh</t>
+  </si>
+  <si>
+    <t>mENU3Iuxhe</t>
+  </si>
+  <si>
     <t>8lv0vbJY4U</t>
   </si>
   <si>
+    <t>kCiV_zttnd</t>
+  </si>
+  <si>
     <t>_aLjTx5BGm</t>
   </si>
   <si>
+    <t>-LRqpiifkZ</t>
+  </si>
+  <si>
+    <t>eCNaC4jWKv</t>
+  </si>
+  <si>
+    <t>tx6J63ey2e</t>
+  </si>
+  <si>
     <t>S5JS_zabnl</t>
   </si>
   <si>
+    <t>V2z8EE0QVv</t>
+  </si>
+  <si>
+    <t>d322X_7IHR</t>
+  </si>
+  <si>
     <t>9oI0wWtSf8</t>
   </si>
   <si>
+    <t>mCmo4ZpkUI</t>
+  </si>
+  <si>
+    <t>T113noFS6C</t>
+  </si>
+  <si>
+    <t>Md-t0ClRpq</t>
+  </si>
+  <si>
     <t>J7KVpZEakd</t>
   </si>
   <si>
     <t>lKaJ9uOfnB</t>
   </si>
   <si>
+    <t>buwb5cnqIJ</t>
+  </si>
+  <si>
+    <t>Gz-lEqxZR2</t>
+  </si>
+  <si>
     <t>ffZTIIa9MZ</t>
   </si>
   <si>
-    <t>27/08/2018</t>
-  </si>
-  <si>
-    <t>5/12/2011</t>
-  </si>
-  <si>
-    <t>15/04/2019</t>
-  </si>
-  <si>
-    <t>10/09/2012</t>
-  </si>
-  <si>
-    <t>20/08/2018</t>
-  </si>
-  <si>
-    <t>18/01/2019</t>
-  </si>
-  <si>
-    <t>26/12/2011</t>
-  </si>
-  <si>
-    <t>2/04/2012</t>
-  </si>
-  <si>
-    <t>20/02/2009</t>
-  </si>
-  <si>
-    <t>22/04/2021</t>
-  </si>
-  <si>
-    <t>6/05/2019</t>
-  </si>
-  <si>
-    <t>4/02/2019</t>
-  </si>
-  <si>
-    <t>2/12/2022</t>
-  </si>
-  <si>
-    <t>30/07/2018</t>
-  </si>
-  <si>
-    <t>17/12/2020</t>
-  </si>
-  <si>
-    <t>25/10/2018</t>
-  </si>
-  <si>
-    <t>06/03/2019</t>
-  </si>
-  <si>
-    <t>22/04/2019</t>
+    <t>AG14xn_Z6F</t>
+  </si>
+  <si>
+    <t>zAY8IgM9z1</t>
+  </si>
+  <si>
+    <t>tXu9TREh_3</t>
   </si>
   <si>
     <t>01/04/2019</t>
@@ -259,30 +277,87 @@
     <t>22/11/2022</t>
   </si>
   <si>
+    <t>21/11/2022</t>
+  </si>
+  <si>
+    <t>11/03/2019</t>
+  </si>
+  <si>
+    <t>15/08/2018</t>
+  </si>
+  <si>
     <t>14/09/2020</t>
   </si>
   <si>
+    <t>14/06/2021</t>
+  </si>
+  <si>
     <t>29/03/2021</t>
   </si>
   <si>
     <t>09/02/2021</t>
   </si>
   <si>
+    <t>26/01/2021</t>
+  </si>
+  <si>
+    <t>18/01/2021</t>
+  </si>
+  <si>
+    <t>11/01/2021</t>
+  </si>
+  <si>
+    <t>24/10/2019</t>
+  </si>
+  <si>
+    <t>24/10/2022</t>
+  </si>
+  <si>
     <t>21/10/2022</t>
   </si>
   <si>
     <t>03/05/2021</t>
   </si>
   <si>
+    <t>26/02/2020</t>
+  </si>
+  <si>
+    <t>20/11/2017</t>
+  </si>
+  <si>
+    <t>09/05/2022</t>
+  </si>
+  <si>
+    <t>13/08/2013</t>
+  </si>
+  <si>
+    <t>18/07/2013</t>
+  </si>
+  <si>
     <t>13/03/2023</t>
   </si>
   <si>
+    <t>21/06/2013</t>
+  </si>
+  <si>
     <t>17/05/2013</t>
   </si>
   <si>
+    <t>26/04/2013</t>
+  </si>
+  <si>
+    <t>10/11/2014</t>
+  </si>
+  <si>
+    <t>04/02/2015</t>
+  </si>
+  <si>
     <t>03/02/2015</t>
   </si>
   <si>
+    <t>28/11/2014</t>
+  </si>
+  <si>
     <t>18/11/2013</t>
   </si>
   <si>
@@ -292,130 +367,154 @@
     <t>14/09/2012</t>
   </si>
   <si>
+    <t>4/06/2012</t>
+  </si>
+  <si>
+    <t>30/05/2012</t>
+  </si>
+  <si>
+    <t>17/08/2019</t>
+  </si>
+  <si>
+    <t>12/03/2012</t>
+  </si>
+  <si>
+    <t>22/03/2013</t>
+  </si>
+  <si>
     <t>20/11/2012</t>
   </si>
   <si>
+    <t>31/10/2012</t>
+  </si>
+  <si>
+    <t>19/01/2017</t>
+  </si>
+  <si>
+    <t>24/06/2016</t>
+  </si>
+  <si>
     <t>23/06/2016</t>
   </si>
   <si>
+    <t>24/01/2017</t>
+  </si>
+  <si>
+    <t>13/03/2015</t>
+  </si>
+  <si>
     <t>30/10/2017</t>
   </si>
   <si>
+    <t>9/10/2017</t>
+  </si>
+  <si>
+    <t>24/05/2017</t>
+  </si>
+  <si>
     <t>26/10/2015</t>
   </si>
   <si>
+    <t>24/06/2022</t>
+  </si>
+  <si>
+    <t>27/05/2015</t>
+  </si>
+  <si>
     <t>17/04/2015</t>
   </si>
   <si>
+    <t>8/04/2015</t>
+  </si>
+  <si>
+    <t>25/03/2015</t>
+  </si>
+  <si>
+    <t>25/02/2015</t>
+  </si>
+  <si>
     <t>17/03/2015</t>
   </si>
   <si>
     <t>17/03/2016</t>
   </si>
   <si>
+    <t>15/02/2017</t>
+  </si>
+  <si>
+    <t>04/02/2017</t>
+  </si>
+  <si>
     <t>27/01/2016</t>
   </si>
   <si>
-    <t>SOJA/CEPEA: Apesar de forte alta do dólar, demanda limita aumento</t>
-  </si>
-  <si>
-    <t>SOJA/CEPEA: Plantio chega à reta final no Brasil</t>
-  </si>
-  <si>
-    <t>SOJA/CEPEA: Negócios são limitados, devido à dificuldade de embarques</t>
-  </si>
-  <si>
-    <t>SOJA/CEPEA: Demanda firme e escassez de oferta mantêm preços elevados</t>
-  </si>
-  <si>
-    <t>SOJA/CEPEA: Cotações seguem em alta</t>
-  </si>
-  <si>
-    <t>OVOS/CEPEA: Poder de compra do avicultor inicia 2019 em queda</t>
-  </si>
-  <si>
-    <t>SOJA/CEPEA: Procura elevada, alta do dólar e problemas logísticos elevam preços domésticos</t>
-  </si>
-  <si>
-    <t>SOJA/CEPEA: Colheita deve começar nesta semana em Mato Grosso</t>
-  </si>
-  <si>
-    <t>SOJA/CEPEA: Soja brasileira valoriza mais de 12% em março</t>
-  </si>
-  <si>
-    <t>SOJA/CEPEA: Mesmo com dólar em queda, Indicador tem maior média mensal desde jan/17</t>
-  </si>
-  <si>
-    <t>FRANGO: Avicultor está no melhor momento no ano</t>
-  </si>
-  <si>
-    <t>SUÍNOS/CEPEA: Quedas no preço do vivo ultrapassam os 20% no mês</t>
-  </si>
-  <si>
-    <t>SOJA/CEPEA: Cotações sobem e liquidez melhora no Brasil</t>
-  </si>
-  <si>
-    <t>MILHO/CEPEA: Com liquidez lenta, atenção se volta a estimativas</t>
-  </si>
-  <si>
-    <t>IPPA/CEPEA: Grãos, pecuária e cana-café elevam IPPA/Cepea em março</t>
-  </si>
-  <si>
-    <t>OVOS/CEPEA: Preço dos insumos favorece avicultor paulista em abril</t>
-  </si>
-  <si>
-    <t>MILHO/CEPEA: Preço fecha janeiro em alta</t>
-  </si>
-  <si>
-    <t>FRANGO/CEPEA: Poder de compra frente ao milho e ao farelo cai pelo 3º mês seguido</t>
-  </si>
-  <si>
-    <t>SOJA/CEPEA: Com baixa liquidez, preços caem no mercado interno</t>
-  </si>
-  <si>
-    <t>IPPA/CEPEA: Índice sobe 4,9% em novembro</t>
-  </si>
-  <si>
-    <t>BOI/CEPEA: Com insumos em alta, produtor está cauteloso quanto a confinamento</t>
+    <t>16/12/2015</t>
+  </si>
+  <si>
+    <t>26/11/2015</t>
+  </si>
+  <si>
+    <t>20/03/2023</t>
+  </si>
+  <si>
+    <t>ARROZ/CEPEA: Com indústria ativa e vendedor recuado, Indicador sobe em março</t>
+  </si>
+  <si>
+    <t>SOJA/CEPEA: Dólar sobe, incentiva novas vendas e eleva preços</t>
+  </si>
+  <si>
+    <t>MILHO/CEPEA: Movimento de queda perde força</t>
+  </si>
+  <si>
+    <t>IPPA/CEPEA: Índice recua em outubro</t>
+  </si>
+  <si>
+    <t>SOJA/CEPEA: Negócios estão aquecidos no Brasil</t>
+  </si>
+  <si>
+    <t>MILHO/CEPEA:  Preços seguem firmes na maior parte das regiões</t>
+  </si>
+  <si>
+    <t>ARROZ/CEPEA: Mercado de arroz tem ritmo lento na primeira quinzena de agosto</t>
+  </si>
+  <si>
+    <t>MILHO/CEPEA: Preços recuam na maior parte das regiões acompanhadas pelo Cepea</t>
+  </si>
+  <si>
+    <t>OVOS/CEPEA: Com valorização de insumos, poder de compra de avicultor recua pelo 5º mês</t>
+  </si>
+  <si>
+    <t>OVOS/CEPEA: Preços recuam pelo 3º mês consecutivo</t>
+  </si>
+  <si>
+    <t>SOJA/CEPEA: Estimativa de maior estoque global pressiona cotações do grão</t>
+  </si>
+  <si>
+    <t>SOJA/CEPEA: Mercado incerto e disparidade entre preços reduzem negócios</t>
+  </si>
+  <si>
+    <t>SOJA/CEPEA: Produtor se retrai e valores voltam a subir</t>
+  </si>
+  <si>
+    <t>OVOS/CEPEA: Valorização dos ovos favorece recuperação do poder de compra do avicultor</t>
+  </si>
+  <si>
+    <t>TRIGO/CEPEA: Liquidez interna é baixa; importação aumenta</t>
+  </si>
+  <si>
+    <t>TRIGO/CEPEA: Baixa oferta interna mantém preço em alta</t>
+  </si>
+  <si>
+    <t>OVOS/CEPEA: Poder de compra do avicultor cai para o menor patamar da história</t>
+  </si>
+  <si>
+    <t>OVOS/CEPEA: Consumo deve continuar elevado em 2021</t>
   </si>
   <si>
     <t>SUÍNOS/CEPEA: Poder de compra aumenta em outubro</t>
   </si>
   <si>
-    <t>TRIGO/CEPEA: Alta do grão é repassada às farinhas</t>
-  </si>
-  <si>
-    <t>SOJA/CEPEA: Caso persista, clima chuvoso pode reduzir qualidade</t>
-  </si>
-  <si>
-    <t>MILHO/CEPEA: Apesar da redução de área, alto estoque pode manter pressão sobre cotações</t>
-  </si>
-  <si>
-    <t>MILHO/CEPEA: Indicador chega a menor patamar em 5 meses</t>
-  </si>
-  <si>
-    <t>ARROZ/CEPEA: Com indústria ativa e vendedor recuado, Indicador sobe em março</t>
-  </si>
-  <si>
-    <t>SOJA/CEPEA: Dólar sobe, incentiva novas vendas e eleva preços</t>
-  </si>
-  <si>
-    <t>MILHO/CEPEA: Movimento de queda perde força</t>
-  </si>
-  <si>
-    <t>IPPA/CEPEA: Índice recua em outubro</t>
-  </si>
-  <si>
-    <t>MILHO/CEPEA: Preços recuam na maior parte das regiões acompanhadas pelo Cepea</t>
-  </si>
-  <si>
-    <t>SOJA/CEPEA: Mercado incerto e disparidade entre preços reduzem negócios</t>
-  </si>
-  <si>
-    <t>SOJA/CEPEA: Produtor se retrai e valores voltam a subir</t>
-  </si>
-  <si>
-    <t>TRIGO/CEPEA: Liquidez interna é baixa; importação aumenta</t>
+    <t>MANDIOCA/CEPEA: Indústrias seguem com dificuldades para se abastecer</t>
   </si>
   <si>
     <t>FRANGO/CEPEA: Poder de compra do avicultor tem novo recuo</t>
@@ -424,15 +523,51 @@
     <t>SOJA/CEPEA: Desvalorização do dólar enfraquece preços no BR</t>
   </si>
   <si>
+    <t>OVOS/CEPEA: Poder de compra aumenta, mesmo com alto preço dos insumos</t>
+  </si>
+  <si>
+    <t>MANDIOCA/CEPEA: Oferta cai e interrompe queda nos preços</t>
+  </si>
+  <si>
+    <t>MANDIOCA/CEPEA: Oferta aumenta, mas preços seguem em patamares elevados</t>
+  </si>
+  <si>
+    <t>SOJA/CEPEA: Com avanço da colheita e baixa demanda externa, preços recuam</t>
+  </si>
+  <si>
+    <t>MILHO/CEPEA: Preço da saca do cereal não cobre custos de produção</t>
+  </si>
+  <si>
+    <t>BOI/CEPEA: Arroba segue em alta em todas as praças acompanhadas</t>
+  </si>
+  <si>
     <t>MILHO/CEPEA: Semeadura segue atrasada, mas safra deve ser recorde</t>
   </si>
   <si>
+    <t>FRANGO/CEPEA: Pela primeira vez no ano, preço do animal vivo reage</t>
+  </si>
+  <si>
     <t>FRANGO/CEPEA: Preço do vivo segue pressionado desde janeiro</t>
   </si>
   <si>
+    <t>FRANGO/CEPEA: Cotações do vivo e da carne seguem em baixa</t>
+  </si>
+  <si>
+    <t>OVOS/CEPEA: Milho e farelo em alta já preocupam avicultores</t>
+  </si>
+  <si>
+    <t>TRIGO/CEPEA: Cotações sobem em janeiro, mas mercado segue retraído</t>
+  </si>
+  <si>
     <t>MILHO/CEPEA: Preços voltam a cair nos portos</t>
   </si>
   <si>
+    <t>SUÍNOS/CEPEA: Poder de compra frente ao milho é o menor desde jul/14</t>
+  </si>
+  <si>
+    <t>SOJA/CEPEA: Desvalorização do dólar enfraquece cotações internas</t>
+  </si>
+  <si>
     <t>SUÍNOS/CEPEA: Queda do vivo e alta do milho reduzem poder de compra</t>
   </si>
   <si>
@@ -445,109 +580,109 @@
     <t>FRANGO/CEPEA: Carne tem preços distintos entre as praças</t>
   </si>
   <si>
+    <t>SOJA/CEPEA: Vendedores se retraem e negócios diminuem</t>
+  </si>
+  <si>
+    <t>TRIGO/CEPEA: Fator climático realça incertezas</t>
+  </si>
+  <si>
+    <t>FRANGO/CEPEA: Média nominal do vivo é recorde; poder de compra se recupera</t>
+  </si>
+  <si>
+    <t>SOJA/CEPEA: Demanda prevalece sobre oferta e preços sobem</t>
+  </si>
+  <si>
+    <t>SUÍNOS/CEPEA: Mercado suinícola segue em queda, mas insumos recuam ainda mais</t>
+  </si>
+  <si>
     <t>MILHO/CEPEA: Agentes estão atentos ao avanço do plantio</t>
   </si>
   <si>
+    <t>TRIGO/CEPEA: Elevação do preço da farinha preocupa indústria alimentícia</t>
+  </si>
+  <si>
+    <t>SUÍNOS/CEPEA: Preços seguem em queda, mas poder de compra do produtor aumenta</t>
+  </si>
+  <si>
+    <t>SOJA/CEPEA: Com menor procura e frete rodoviário elevado, valores caem no BR</t>
+  </si>
+  <si>
+    <t>FRANGO/CEPEA: Altas nos preços do vivo seguem intensas</t>
+  </si>
+  <si>
     <t>SUÍNOS/CEPEA: Em SP, poder de compra frente ao milho cresce 20%</t>
   </si>
   <si>
+    <t>TRIGO/CEPEA: Com realização de leilões, preços reagem no RS e SP</t>
+  </si>
+  <si>
+    <t>FRANGO/CEPEA: Preço da carne recua, mesmo com vivo estável</t>
+  </si>
+  <si>
+    <t>OVOS/CEPEA: Preço cai, mas poder de compra de avicultor continua elevado</t>
+  </si>
+  <si>
     <t>MILHO/CEPEA: Vendedores reduzem oferta e valores seguem em alta</t>
   </si>
   <si>
+    <t>MILHO/CEPEA: Diferença entre preço pedido e ofertado reduz liquidez interna</t>
+  </si>
+  <si>
     <t>OVOS/CEPEA: Oferta restrita e aumento da demanda sustentam preços</t>
   </si>
   <si>
+    <t>ARROZ/CEPEA: Produtor recuado e indústria ativa impulsionam preço do casca em junho</t>
+  </si>
+  <si>
+    <t>ARROZ/CEPEA: Demanda segue enfraquecida e preços, estáveis</t>
+  </si>
+  <si>
+    <t>MILHO/CEPEA: Exportação tem alta de mais de 60% em maio</t>
+  </si>
+  <si>
     <t>SOJA/CEPEA: Preços sobem; clima melhora e favorece cultivo</t>
   </si>
   <si>
+    <t>FRANGO/CEPEA: Poder de compra recua em junho</t>
+  </si>
+  <si>
+    <t>OVOS/CEPEA: Com nova queda de preço, alívio vem de insumos mais baratos</t>
+  </si>
+  <si>
     <t>SUÍNOS/CEPEA: Preços do animal vivo e da carne seguem em queda</t>
   </si>
   <si>
+    <t>MILHO/CEPEA: Colheita e plantio estão na reta final; mercado busca direção</t>
+  </si>
+  <si>
+    <t>MILHO/CEPEA: Perspectiva de aumento das exportações sustenta valores</t>
+  </si>
+  <si>
+    <t>TRIGO/CEPEA: Liquidez recua, mas cotação segue firme</t>
+  </si>
+  <si>
     <t>TRIGO/CEPEA: Dólar em alta e moinhos ativos elevam cotações do grão</t>
   </si>
   <si>
     <t>SUÍNOS/CEPEA: Alta no preço do milho segue pressionando poder de compra</t>
   </si>
   <si>
+    <t>SOJA/CEPEA: Queda nos preços é limitada por dólar elevado</t>
+  </si>
+  <si>
+    <t>SUÍNOS/CEPEA: Vivo e carne continuam desvalorizados</t>
+  </si>
+  <si>
     <t>OVOS/CEPEA: Oferta recua, pressionada pelas altas dos insumos</t>
   </si>
   <si>
-    <t>precos soja subiram mercado brasileiro ultimos dias pesquisadores afirmam apesar forte valorizacao dolar frente real demanda enfraquecida limitou avancos internos segundo traders consultados praticamente nao procura externa oleaginosa brasileira ultimos dias deve tambem expressiva queda contratos futuros cme group bolsa chicago devido boas condicoes lavouras norteamericanas cenario alimenta expectativas safra recorde temporada indicador esalqbmfbovespa soja paranagua pr subiu leve agosto r saca kg nessa sextafeira indicador esalq parana aumento comparativo r sc kg</t>
-  </si>
-  <si>
-    <t>plantio soja caminhando final negociacoes sido lentas mercado brasileiro segundo agentes colaboradores aproximadamente area soja ja semeada regioes mato grosso mato grosso sul parana faltam cerca serem semeados estado sao paulo area ja plantada goias cerca rio grande sul santa catarina quanto precos mercado brasileiro sido praticamente nominais novembro dezembro indicador esalqbmfbovespa produto transferido armazens porto paranagua dolar moeda prevista contratos futuros bmfbovespa subiu expressivos fechando us sc kg sextafeira moeda nacional indicador registrou ligeira baixa finalizou r sc quanto media ponderada regioes paranaenses refletida indicador esalq fechou r sc sexta queda relacao sextafeira anterior</t>
-  </si>
-  <si>
-    <t>ritmo exportacoes soja derivados diminuiu nesta semana devido dificuldade embarque alguns traders consultados indicam chuvas ocorridas ultimas semanas atrasaram programacao escoamento principais portos brasileiros santos sp paranagua pr rio grande rs cenario diminuiu cotas armazens portuarios tradings pretendiam enviar novos lotes portos exportacoes limitadas tambem atraso navios especialmente santos neste caso lotes deveriam escoados duas ultimas semanas prorrogados segunda quinzena deste mes regiao matopiba acordo levantamento precipitacoes seguem atrasando colheita limitando comercializacoes quanto precos indicador esalqbmfbovespa soja paranagua recuou r saca kg dia comparativo indicador esalq parana baixa r sc kg nessa sexta fonte wwwesalquspbr</t>
-  </si>
-  <si>
-    <t>cotacoes soja derivados seguem elevados estados unidos brasil devido oferta restrita demanda firme cultivo soja deve ganhar area proxima safra america sul pode proporcionar producao recorde caso clima colabore relacao proxima temporada produtores brasileiros adiantaram compras insumos estao cautelosos quanto momento iniciar semeadura segundo colaboradores grande parte produtores atenta previsoes climaticas proximos meses modo evitar lavouras sofram falta umidade periodo desenvolvimento mercado spot nacional precos permanecem firmes porem praticamente nominais parcial setembro agosto setembro indicador esalqbmfbovespa produto transferido armazens porto paranagua dolar moeda prevista contratos futuros bmfbovespa alta fechando us sc kg nessa quintafeira moeda nacional indicador tambem registrou elevacao r saca kg nessa quinta media ponderada regioes paranaenses refletida indicador esalq r sc kg quintafeira aumento acumulado mes</t>
-  </si>
-  <si>
-    <t>menor excedente interno safra baixa oferta caminhoes grande parte sojicultores consultados prefere guardar oleaginosa estoque comercializar partir outubro sinaliza paridade exportacao atrativa apesar colheita americana agentes colaboradores relatam logistica entrega setembro ja praticamente tomada impedindo novas grandes negociacoes entrega neste periodo geral demanda externa grao brasileiro segue aquecida cenario mantido premios exportacao brasil alta adicionado maior taxa cambio precos soja seguem elevados indicador esalqbmfbovespa soja paranagua pr avancou agosto r saca kg nessa sextafeira comparativo indicador esalq parana subiu r sc kg elevacao precos domesticos deve tambem valorizacao dolar frente real</t>
-  </si>
-  <si>
-    <t>acordo pesquisadores oferta elevada segue pressionando cotacoes ovos impactado negativamente poder compra avicultor postura paulista frente principais insumos utilizados alimentacao poedeiras milho farelo soja parcial deste mes quantidade cereal produtor consegue comprar venda ovos brancos menor toda serie iniciada maio ja sobre quantidade derivado soja menor desde dezembro fonte</t>
-  </si>
-  <si>
-    <t>precos soja subiram mercado brasileiro ultimos dias impulsionados valorizacao dolar firme demanda atraso embarques grao atraso deve baixa disponibilidade caminhoes gerado filas navios portos agentes consultados indicam frete rodoviario saltou r tonelada inicio fevereiro aproximadamente r t primeira semana marco atraso colheita entrega soja volume disponivel mercado spot segue baixo elevando cotacoes indicador esalqbmfbovespa paranagua subiu fevereiro marco fechando r sc sextafeira indicador esalq parana registrou alta mesma comparacao r sc kg dia fonte</t>
-  </si>
-  <si>
-    <t>colheita safra deve comecar nesta semana mato grosso devendo abrir trabalhos parana maquinas devem ir campo cerca quinze dias falta chuvas segunda quinzena novembro boa parte dezembro algumas regioes centrooeste sudeste praticamente todas regioes agricolas importantes sul deve reduzir produtividade argentina trabalhos cultivo estao praticamente suspensos tambem falta chuva dados oferta demanda mundial usda ministerios agricultura estados unidos divulgados inicio dezembro ja sinalizavam estoques passagens safra devem reduzir levando relacao estoqueconsumo menor tres safras mercado brasileiro negociacoes soja derivados estao bastante lentas neste final ano negociacoes sido registradas apenas pequenos lotes interior pais representando preco medio ponderado regioes paranaenses indicador esalq fechou r sc nessa sexta ligeira baixa sobre sexta anterior porto paranagua devido baixa liquidez indicador esalqbmfbovespa representa cotacao media soja posta armazem desse porto sido frequentemente arbitrado r sc desde dia dezembro</t>
-  </si>
-  <si>
-    <t>indicador esalq soja reflete forma ponderada precos estado parana altas praticamente diarias longo marco caiu somente dia chegando casa r saca kg marco alta alcancou referente soja grao transferida armazens porto paranagua indicador esalqbmfbovespa acumulou aumento mes r saca kg sextafeira segundo pesquisadores ritmo refletido boa demanda produto brasileiro supera oferta disponivel neste periodo final safra</t>
-  </si>
-  <si>
-    <t>precos soja derivados estao enfraquecidos mercado brasileiro reflexo desvalorizacoes dolar frente real cautela compradores quanto novas aquisicoes conta expectativas estoques finais elevados dez maior area semeada safra ultima sextafeira dolar fechou brl baixa sete dias assim medias indicadores parana paranagua mes sao maiores desde fevereiro janeiro respectivamente termos reais igpdi junho conforme colaboradores altas frete rodoviario devido maior concorrencia transporte milho limitaram recuo soja ultimos dias comparandose media parcial julho ate dia mes anterior indicador esalq parana subiu significativos esalqbmfbovespa paranagua</t>
-  </si>
-  <si>
-    <t>diante altas precos frango vivo desde inicio ano desvalorizacoes principais insumos utilizados producao milho farelo soja avicultor paulista encontra situacao favoravel deste ano interior estado sao paulo frango vivo acumula aumento parcial deste mes negociado r kg nessa quintafeira valorizacao decorre menor producao avicultores visando controlar oferta periodo saca kg milho caiu campinas sp dessa forma avicultor melhora poder compra ultima quintafeira venda quilo frango rendeu kg milho farelo soja recuo acumulado fevereiro fazendo poder compra produtor aumentasse periodo quinta venda quilo vivo avicultor conseguiu comprar kg farelo</t>
-  </si>
-  <si>
-    <t>movimento baixa precos suino vivo persiste praticamente todas regioes pesquisadas correr deste mes desvalorizacoes animal chegam pracas sp pr recuos acontecem tanto mercados dirigidos consumidor domestico quanto exportacao vez insumos importantes atividade milho farelo soja mantido estaveis resultando perda poder compra suinocultores intensas desvalorizacoes vivo nessa parcial agosto julho agosto observadas regioes sao paulo parana sao jose rio preto sp exemplo quilo animal ja recuou indo media r kg nessa quintafeira regiao paranaense apresentou queda acentuada pato branco animal comercializado media r kg nessa quinta</t>
-  </si>
-  <si>
-    <t>precos soja estao alta mercados brasileiro internacional sustentados preocupacoes cultivo lento estados unidos possivel diminuicao produtividade brasil segundo pesquisadores produtores voltam focar comercializacoes grao prontaentrega sido estimuladas proximidade valores compradores vendedores vale lembrar semana passada agentes apenas cumprindo contratos realizados ano passado entrega abril maio alem disso rumor maior demanda parte china elevou precos restricao oferta norteamericana china pode intensificar compras brasil parcial maio ate dia indicador esalqbmfbovespa produto transferido porto paranagua subiu finalizando us sc kg moeda nacional indicador avanco periodo finalizando r sc nessa sexta quanto media ponderada regioes paranaenses refletida indicador esalq elevacao parcial mes fechando r sc sexta maio</t>
-  </si>
-  <si>
-    <t>comercializacao milho segue lenta mercado brasileiro produtores consultados dado prioridade negociacoes soja visto precos oleaginosa estao firmes conta problemas transporte ate porto paranagua alem disso vendedores realizado contratos envolvendo cereal segunda safra diante ritmo lento mercado atencao agentes consultados voltada divulgacoes dados safra brasil estimativas agregadas temporada mundial brasil conab elevou ligeiramente producao safra verao enquanto usda surpreendeu mercado dados indicando producao recorde estados unidos maio indicador esalqbmfbovespa campinassp valores prazo sao convertidos vista taxa desconto cdi subiu fechando r sc kg segundafeira considerada taxa desconto npr regiao campinas preco medio vista nessa segunda r sc kg aumento comparativo segundafeira anterior</t>
-  </si>
-  <si>
-    <t>fevereiro marco ippa indice precos produtor grupos produtos agropecuarios subiu termos nominais segundo pesquisadores movimento atrelado variacoes positivas observadas ippagraos ippapecuaria ippacanacafe ja ippahortifruticolas caiu desempenho indice graos deve avanco valores milho algodao trigo soja arroz casca unico desvalorizar mes caso pecuaria resultado indice impulsionado alta precos nominais frango vivo boi gordo ovos contrapondose quedas observadas suino vivo leite aumentos precos nominais canadeacucar cafe respondem desempenho indice composto ambos produtos ja hortifruticolas resultado negativo reflete quedas observadas precos nominais tomate banana laranja mesma comparacao ipaogdi produtos industriais calculado divulgado fgv registrou alta logo fevereiro marco precos agropecuarios cairam pouco frente industriais economia fonte</t>
-  </si>
-  <si>
-    <t>marco abril ovos brancos tipo extra negociados bastos sp registraram ligeira valorizacao outro lado principais insumos utilizados alimentacao poedeiras milho farelo soja retracao precos elevou poder compra avicultores paulistas patamares nao observados desde outubro abril caixa duzias ovos brancos tipo extra preco medio r bastos ate feriado religioso sextafeira santa valores recebidos produtores registravam tendencia altista passando recuar partir dia fechando r cx ultimo dia util abril acordo colaboradores consultados expectativa proximidade periodo recebimento salarios dia maes vendas ovos aquecam elevando cotacoes fonte wwwesalquspbr</t>
-  </si>
-  <si>
-    <t>precos milho acumularam ligeiro aumento janeiro elevacao ritmo exportacoes ultimas semanas menor interesse vendedores consultados comercializar cereal sustentaram cotacoes avanco colheita soja agentes priorizam comercializacao oleaginosa mantendo ritmo lento negociacao cereal produtores consultados limitaram ofertas novos negocios espera valorizacoes expressivas alem disso irregularidade chuvas deixado produtores cautelosos fortalece recuo vendedor lado comprador agentes aguardam avanco colheita maiores definicoes produtividade assim mantem apenas aquisicoes pequenos lotes fazer estoques curto prazo indicador esalqbmfbovespa regiao campinassp subiu dezembro janeiro fechando r saca kg dia especificamente janeiro fevereiro indicador subiu fonte</t>
-  </si>
-  <si>
-    <t>precos medios frango vivo cairam outubro novembro segundo pesquisadores valores pressionados aumento oferta produtos avicolas mercado interno outro lado cotacoes principais insumos atividade milho farelo soja avancaram periodo diante desse cenario calculos mostram poder compra avicultor estado sao paulo frente insumos caiu outubro novembro pesquisadores ressaltam terceiro mes seguido piora relacao troca fonte</t>
-  </si>
-  <si>
-    <t>precos soja estao queda mercado brasileiro acordo levantamento devido desvalorizacao dolar frente real impacta diretamente paridade exportacao deixando menos atrativas vendas oleaginosa vendedores consultados capitalizados compradores objetivando aproveitar momento valores baixos tambem maior disparidade cotacoes desses agentes reduzindo liquidez interna assim dia indicador esalqbmfbovespa paranagua fechou r saca kg abaixo registrado dia indicador esalq parana tambem recuou julho r sc kg dia</t>
-  </si>
-  <si>
-    <t>novembro ippa indice precos produtor grupos produtos agropecuarios avancou termos nominais frente outubro resultado indice geral reflete variacoes positivas observadas todos grupos produtos destaque ippagraos registrou alta seguido ippapecuaria ippacana cafe forma sutil ippahortifruticolas elevacao excecao preco arroz todos itens compoem indice graos subiram especial milho soja pecuaria desempenho indice influenciado principalmente valorizacoes boi suinos sutilmente frangos ovos ja altas precos canadeacucar cafe impulsionaram desempenho indice composto produtos fim hortifruticolas elevacao impulsionada avanco precos batata menor intensidade uva laranja mesma comparacao ipaogdi produtos industriais calculado divulgado fgv subiu logo outubro novembro precos agropecuarios valorizaram frente precos industriais economia fonte</t>
-  </si>
-  <si>
-    <t>neste momento antecede periodo seca pecuaristas corte planejado quanto volume animais vao confinar proximas semanas conforme colaboradores atencoes produtores estao voltadas atuais precos boi magro principalmente milho farelo soja importantes insumos racao estao alta outro termometro utilizado mercado vem influenciando certa cautela alguns produtores sao precos boi gordo mercado futuro b antiga bmfbovespa proximos vencimentos apontam quedas valores arroba</t>
-  </si>
-  <si>
-    <t>elevacao precos suino vivo recuos cotacoes milho farelo soja neste mes poder compra suinocultores sao paulo oeste catarinense favoravel segundo pesquisadores mercado suinicola oferta reduzida animais abate bom resultado exportacoes correr segundo semestre elevado preco animal quanto milho acordo equipe graos motivos quedas sao maior disponibilidade mercado domestico retracao compradores finalmente farelo ainda acordo equipe graos demanda enfraquecida vem pressionando negociacoes fonte</t>
-  </si>
-  <si>
-    <t>elevacoes trigo grao sido repassadas farinhas ainda poucos sete diferentes farinhas acompanhadas apenas duas premistura massas frescas desvalorizaram semana passada quanto farelo demanda pouco aquecida devido fortes avancos cotacoes milho relacao trigo grao cotacoes tambem estao alta impulsionadas periodo entressafra alem disso maior custo importacao atrasos embarques cereal argentino direcionado compradores mercado domestico volume disponivel mercado nacional ainda baixo mantem produtores firmes precos pedidos muitos estao fazendo caixa venda soja milho</t>
-  </si>
-  <si>
-    <t>recentes chuvas atrapalhado trabalhos campo gerado preocupacoes quanto qualidade soja acordo informacoes caso cenario volume elevado precipitacoes luminosidade reduzida persista graos ainda estao lavouras podem prejudicados especialmente regioes sudeste centrooeste matopiba quanto negocios diante maior incerteza quanto produtividade atual temporada sojicultores brasileiros voltaram reduzir vendas menor interesse negociacao tambem deve queda valores futuros cme group bolsa chicago reducao premios exportacao brasil desvalorizacao cambial demanda relativamente estavel fonte</t>
-  </si>
-  <si>
-    <t>apos safra brasileira recorde consequente queda precos internos area milho temporada deve menor desde acordo colaboradores alem menor rentabilidade cultura ultima safra reducao area tambem atrelada atraso colheita soja algumas regioes brasileiras apesar disso alto estoque passagem deve manter elevada disponibilidade interna cereal termos mundiais menor produtividade deve reduzir oferta milho enquanto transacoes internacionais devem crescer pode favorecer exportacoes brasileiras</t>
-  </si>
-  <si>
-    <t>oferta superior demanda mantido precos milho queda maior parte regioes acompanhadas campinas sp valores voltaram operar proximos patamares observados novembro ano passado abril indicador esalqbmfbovespa campinas sp caiu r sc kg quintafeira menor patamar nominal desde meados novembro geral ritmo negocios limitado tendo vista disparidade ofertas compradores pedidos vendedores alem disso alguns produtores dado preferencia comercializar soja vale lembrar cotacao oleaginosa firme favorecida altas dolar precos externos campo clima segue favoravel desenvolvimento lavouras milho pode resultar antecipacao colheita fonte</t>
+    <t>OVOS/CEPEA: Consumo de final de ano se aquece e eleva preços</t>
+  </si>
+  <si>
+    <t>SUÍNOS/CEPEA: Preço do vivo reage na semana; poder de compra diminui no ano</t>
+  </si>
+  <si>
+    <t>SOJA/CEPEA: Volume de chuvas diminui, e colheita avança no BR</t>
   </si>
   <si>
     <t>compradores ativos vendedores mercado arroz casca rio grande sul marco principalmente segunda quinzena segundo colaboradores industrias necessidade repor estoques ofertaram valores superiores novos lotes arroz novo safra lado produtor orizicultores permaneceram recuados atentos condicoes climaticas estado atividades colheita assim vendas efetivadas devido necessidade fazer caixa outros vez optaram negociar gado soja nesse cenario indicador arroz casca esalqsenarrs graos inteiros acumulou alta mes passado fechando r sc kg dia fonte wwwesalquspbr</t>
@@ -562,33 +697,105 @@
     <t>outubro ippa indice precos produtor grupos produtos agropecuarios caiu relacao setembro termos nominais influenciado quedas observadas ippacanacafe ippapecuaria ippagraos cujas variacoes negativas respectivamente ja ippahortifruti avancou resultado ippapecuaria deveu queda precos nominais leite frango vivo boi gordo ovos caso leite baixa atrelada enfraquecimento demanda aumento oferta funcao incremento producao aumento importacoes caso carnes avicolas bovinas pressao sobre valores veio sobretudo crescimento oferta animais grupo ippagraos recuos precos algodao pluma soja reflexo observado mercado externo quanto resultado ippacanacafe deveu queda precos ambos produtos especificamente caso cafe clima favoravel vem gerando expectava boa producao consequentemente quedas precos fim sentido oposto temse resultado altista observado ippahortifruti devido comportamento valores tomate banana batata uva laranja mesma comparacao ipaogdi produtos industriais calculado divulgado fgv registrou queda logo setembro outubro precos agropecuarios cairam frente industriais economia fonte</t>
   </si>
   <si>
+    <t>comercializacao soja grao aquecida mercado brasileiro cenario atrelado demanda firme sobretudo externa maior necessidade venda parte sojicultor neste caso pesquisadores ressaltam volume remanescente grao safra elevado expectativa producao recorde temporada fonte</t>
+  </si>
+  <si>
+    <t>menor producao safra verao expectativa disponibilidade restrita proximas semanas mantem produtores milho consultados elevando valores venda agricultores tambem estao concentrados finalizacao colheita soja alguns casos semeio segunda safra milho compradores consultados vez adquirem novos lotes spot ha necessidade repor estoques neste caso precisam pagar precos superiores conseguir fechar negocios diante disso movimento alta cotacoes segue firme maior parte regioes acompanhadas sobretudo consumidoras sao paulo parana marco especificamente indicador esalqbmfbovespa subiu fechando r sc sextafeira fonte wwwesalquspbr</t>
+  </si>
+  <si>
+    <t>negociacoes arroz casca rio grande sul apresentaram ritmo lento nesta primeira quinzena agosto algumas industrias consultadas priorizaram apenas compras arroz depositado armazens devido dificuldades repasse altas casca beneficiado enquanto outras mercado trabalhando apenas produto ja comprado alem disso algumas beneficiadoras adquiriram novos lotes arroz livre armazenados propriedades rurais repor estoques lado vendedor alguns orizicultores disponibilizaram lotes devido necessidade fazer caixa atender compromissos bancarios outros optaram negociar outras commodities soja exemplo agosto indicador arroz casa esalqsenarrs graos inteiros caiu leve fechando r sc kg dia</t>
+  </si>
+  <si>
     <t>menor interesse compradores indicam ter estoques curto prazo pressionado valores milho maior parte regioes acompanhadas praca campinas sp base indicador esalqbmfbovespa saca kg milho registrou queda setembro fechando r nessa sextafeira acumulado setembro ate dia baixa porem especificamente final semana passada valores subiram devido retracao produtores resistentes negociacoes envolvendo grandes lotes campo produtores brasileiros voltam ficar atentos clima tendo vista tempo seco pode dificultar semeio soja outubro consequentemente atrasar plantio milho segunda safra sul falta chuvas ja preocupa agentes quanto desenvolvimento temporada verao fonte</t>
   </si>
   <si>
+    <t>poder compra avicultor postura segue queda neste mes apesar ligeira valorizacao ovos primeira semana agosto porque cotacoes principais insumos consumidos atividade milho farelo soja estao patamares bastante elevados aumentando relacao troca ovos produtos vale lembrar quinto mes consecutivo queda poder compra avicultor recuos mensais vem sendo registrados desde abril segundo colaboradores cenario preocupado avicultores ja reportam dificuldades obter margens positivas fonte</t>
+  </si>
+  <si>
+    <t>leve valorizacao ultima semana julho precos ovos cairam media mes acumulando tres periodos consecutivos recuos segundo dados pandemia covid impactos poder compra populacao gradativamente reduzido liquidez produto principais regioes consumidoras pressionando cotacoes demanda desaquecida descartes poedeiras velhas devem antecipados acordo colaboradores tentativa diminuir oferta ovos impulsionar precos vez margens setor estado estreitas devido elevados patamares precos principais insumos consumidos atividade milho farelo soja fonte</t>
+  </si>
+  <si>
+    <t>precos soja cairam brasil estados unidos longo semana passada influenciados estimativas usda indicando maior estoque mundial safras pesquisadores ressaltam desvalorizacao dolar frente real contudo limitou queda precos internacionais medida deixa oleaginosa norteamericana atrativa reduziu liquidez brasil diante disso junho indicador esalqbmfbovespa paranagua caiu fechando r sc kg sextafeira comparativo indicador esalq parana cedeu indo r sc kg fonte</t>
+  </si>
+  <si>
     <t>liquidez mercado soja derivados segue baixa tanto contratos spot quanto termo principalmente incertezas quanto implementacao tabelamento fretes tensao comercial estados unidos china ampliado diferenca valores pedidos vendedores ofertados compradores dificultando fechamento novos negocios oscilacoes premios exportacao cambio assim expectativa continuidade valorizacoes observadas ultimas semanas tambem reduziram negociacoes contratos termo spot segundo colaboradores logistica tomada recebimento lotes fixados antecipadamente tambem impedindo comercializacao grandes volumes maioria efetivacoes ocorre completar cargas visto ha navios previstos sair portos proximos dias</t>
   </si>
   <si>
     <t>precos soja subiram mercado brasileiro semana passada movimento atrelado valorizacoes externa cambial retracao sojicultores segundo pesquisadores metade safra ja comercializada agora produtores preferem colher armazenar grao expectativa vender oleaginosa valores maiores meses posteriores mercado spot indicador esalqbmfbovespa paranagua subiu marco indo r sc kg sextafeira indicador esalq parana avancou mesma comparacao r sc kg sexta fonte</t>
   </si>
   <si>
+    <t>consecutivas altas precos ovos fevereiro favoreceram recuperacao poder compra avicultor postura frente principais insumos alimentacao consumidos atividade milho farelo soja janeiro relacao troca proteina insumos maior serie historica iniciada produto entanto apesar valorizacao ovos neste mes cenario ainda desfavoravel produtor cujo poder compra permanece abaixo observado longo primeiro semestre fonte</t>
+  </si>
+  <si>
     <t>baixa disponibilidade trigo ritmo lento negocios mercado brasileiro levaram industrias intensificarem importacoes cereal janeiro mercado lotes colaboradores relataram negocios pontuais intuito liberar espaco armazens entrada safra soja lado consumidor moinhos estao atentos chegada trigo importado proximas semanas dados secex apontam total adquirido janeiro mil toneladas volume superior dezembro abaixo janeiro fonte</t>
   </si>
   <si>
+    <t>precos trigo seguem alta mercado brasileiro segundo pesquisadores sustentacao vem baixa disponibilidade domestica maior interesse ainda pontual compradores alem disso valorizacao dolar tambem influencia cotacoes cereal medida encarece importacoes quanto negociacoes estao lentas mercado balcao colaboradores relataram sustentacao vem maior intencao compra parte cooperativas intuito estimular produtores comercializar assim liberar espaco armazens safra soja ja mercado lotes vendedor segue retraido dificultando aquisicao materiaprima parte moinhos necessitam repor estoques fonte</t>
+  </si>
+  <si>
+    <t>janeiro precos principais insumos consumidos avicultura postura milho farelo soja voltaram elevar cenario somado menores precos pagos caixa ovos comerciais pressionou poder compra avicultor postura menor patamar ja registrado serie historica iniciada produto fonte</t>
+  </si>
+  <si>
+    <t>economia brasileira pode iniciar recuperacao gradual deve favorecer consumo ovos precos baixos frente demais proteinas origem animal alem disso possivel vacinacao imunizacao contra covid consequente reducao efeitos pandemia podem permitir retorno aulas forma presencial bem outros eventos tambem deve alavancar consumo dados associacao brasileira proteina animal abpa indicam producao brasileira ovos pode aumentar frente projetado passando bilhoes unidades consumo vez pode unidades per capita durante ano previsto outro lado custos producao devem continuar sendo grande entrave setor vez valores dois principais insumos consumidos atividade milho farelo soja devem manter elevados neste ano tendo vista estoques baixos aquecidas demandas interna externa produtos fonte</t>
+  </si>
+  <si>
+    <t>poder compra suinocultor aumentado correr deste mes acordo informacoes devido precos suino vivo estarem alta intensa registrado cotacoes milho farelo soja quanto suino ritmo aquecido exportacoes proteina segue impulsionando procura animais consequentemente valores relacao insumos precos estao alta devido demanda aquecida sobre exportacoes tres primeiras semanas outubro media diaria exportacao carne suina in natura mil toneladas aumento frente setembro segundo relatorio secex assim dias uteis embarcadas mil toneladas ritmo mantiver serao exportadas mil t ate encerramento outubro fonte</t>
+  </si>
+  <si>
+    <t>disponibilidade lavouras serem colhidas segue baixa parte agricultores postergado comercializacao raiz mandioca segundo pesquisadores agentes estao focados atividades plantio mandioca eou soja tratos culturais alem disso chuvas registradas alguns dias ultima semana tambem reforcaram menor oferta raiz tendo vista dificultam colheita lado demanda maior interesse industrias fecula farinha aumentar quantidades mandioca processadas baixa oferta muitas empresas buscaram abastecer areas distantes pouco sucesso assim sido maior disputa materiaprima diferentes regioes produtoras fonte</t>
+  </si>
+  <si>
     <t>setembro parcial outubro precos frango vivo registrado queda segundo pesquisadores pressao vem aumento oferta animais outro lado valores principais insumos cadeia avicola milho farelo soja apresentam estabilidade avancos respectivamente nesse contexto poder compra avicultor frente insumos vem recuando outubro tratase segundo mes seguido piora relacao troca avicultor fonte</t>
   </si>
   <si>
     <t>precos soja recuaram mercado brasileiro semana passada segundo pesquisadores pressao veio desvalorizacao dolar frente real reducao demanda interna neste caso muitas industrias trabalham oleaginosa ja contratada enquanto outras unidades sul pais indicam importar materiaprima paraguai outro lado demanda externa aquecida acabou limitando movimento queda precos brasil abril indicadores esalqbmfbovespa paranagua esalq parana recuaram respectivamente indo r r sc kg sextafeira fonte</t>
   </si>
   <si>
+    <t>baixa disponibilidade ovos somada incertezas mercado conta pandemia coronavirus elevou significativamente cotacoes proteina atingiram patamar recorde acordo dados dessa forma altos valores principais insumos utilizados atividade milho farelo soja poder compra avicultor postura aumentou media parcial abril especificamente semana passada cotacoes ovos registraram apenas pequenas alteracoes permanecendo estaveis maioria regioes acompanhadas apesar disso vendas diminuiram fonte</t>
+  </si>
+  <si>
+    <t>diminuicao ritmo colheita comercializacao ja vinha ocorrendo duas ultimas semanas fevereiro intensificou fevereiro todas regioes acompanhadas resultado precos queda desde primeira quinzena dezembro registraram altas periodo cenario deve retracao parte agricultores consultados nao considera viavel comercializar atuais patamares tempo ha produtores priorizaram outras atividades colheita soja demanda industrial outro lado fortalecido acordo pesquisas principalmente conta expectativa retomada comercializacao derivados apos carnaval fonte</t>
+  </si>
+  <si>
+    <t>ritmo colheita aumentou ultimos dias devido condicoes climaticas favoraveis encerramento plantio mandioca soja maior interesse parte produtores capitalizar apesar disso oferta ainda considerada bastante baixa periodo todas regioes acompanhadas permanecendo abaixo demanda industrial mantendo precos patamares elevados nesse cenario media semanal prazo tonelada mandioca posta fecularia ficou r r grama amido balanca hidrostatica kg novembro acima media anterior frente periodo ano passado elevacao valores atualizados deflacionamento igpdi outubro</t>
+  </si>
+  <si>
+    <t>precos soja registraram baixa ultimos dias segundo informacoes abril maio indicador esalq parana caiu fechando r saca kg sextafeira indicador esalqbmfbovespa paranagua pr recuou r sc kg dia acordo pesquisadores pressao veio menor demanda externa sobretudo china evolucao colheita america sul alem disso baixo volume negociado oleaginosa safra brasil falta espaco armazens grandes regioes produtoras pais vem gerando expectativas maior oferta curto prazo fonte</t>
+  </si>
+  <si>
+    <t>elevada oferta atual expectativa estoques finais recordes pressionado precos milho brasil centrooeste parana atuais valores saca estao abaixo minimo estipulado governo excecao sudoeste parana ponta grossa pr valores minimos definidos governo prevalecem neste segundo semestre sao r saca kg estados goias parana mato grosso sul r saca kg mato grosso alem disso segundo calculos realizados equipe custos atual valor saca milho nao cobre custos producao assim produtores estao negociando restante safra soja estocando milho espera maior remuneracao colaboradores indicam necessaria continuidade intervencoes federais meio leiloes compra opcoes pepro escoar produto manter renda produtor</t>
+  </si>
+  <si>
+    <t>baixa oferta animais abate nesta entressafra impulsionado cotacao arroba todas regioes acompanhadas estado sao paulo indicador boi gordo esalqbmfbovespa media ponderada quatro regioes aumentou julho fechando r nessa quartafeira mercado reposicao indicador bezerro esalqbmfbovepa animal nelore meses mercado sulmatogrossense fechou r quarta vale lembrar ainda maior patamar nominal ja verificado considerandose serie historica iniciada enquanto parte pecuaristas mostra preocupada diante elevados precos bezerro tambem boi magro apesar disso pesquisadores indicam cenario pode melhor favorecido queda precos alimentacao milho farelo soja segundo dados compra animais alimentacao correspondem coe custo operacional efetivo</t>
+  </si>
+  <si>
     <t>apesar atrasos semeadura segunda safra milho brasil dados oficias seguem apontando producao nacional recorde ja argentina novos ajustes negativos estimativas levaram reducao producao mundial ressaltase so nao caiu intensidade conta maior colheita brasil manutencao producao estados unidos neste contexto pesquisadores indicam enquanto produtores estao focados trabalhos campo consumidores nacionais adquirem novos lotes apenas ha necessidade recompor estoques ainda assim alguns demandantes acabam tendo dificuldades aquisicoes conta questoes logisticas avanco colheita soja frete oleaginosa certa prioridade fonte</t>
   </si>
   <si>
+    <t>reducao oferta animais fez cotacoes frango vivo aumentassem primeira vez ano maioria regioes acompanhadas acordo produtores maior procura tambem deu certa colaboracao reajustes positivos segundo pesquisadores segmento carnes precos frango congelado tambem reagem maioria pracas resfriado ainda mantem predominantemente queda mercado insumos farelo soja segue alta refletindo demanda aquecida restricao vendedora maior taxa cambio</t>
+  </si>
+  <si>
     <t>oferta frango vivo continua maior demanda pressionado precos vem caindo desde inicio ano maioria regioes acompanhadas relacao segmento carne maior liquidez inicio mes ocasiao dia maes pagamento salario nesta semana ritmo comercializacao voltou diminuir reduzindo cotacoes mercado insumos estimativas apontam producao milho cada vez maior safra inverno pode fazer cotacoes grao recuem forca medio prazo enquanto segundo dados precos seguem firmes relacao farelo soja demanda internacional derivado aquecida ultimos dias</t>
   </si>
   <si>
+    <t>valores frango vivo carne seguem registrando quedas expressivas segundo colaboradores mercado ainda enfraquecido nesta semana visto liquidez tradicionalmente diminui final mes sucessivas baixas refletem oferta acima demanda carne impacta tambem segmento frango vivo relacao principais insumos usados atividade milho farelo soja precos tambem estao queda nao suficiente sustentar poder compra avicultor paulista</t>
+  </si>
+  <si>
+    <t>recentes valorizacoes ovos altas precos principais insumos utilizados setor avicola destaque milho farelo soja comecam deixar avicultores postura alerta relacao rentabilidade atividade porque apesar demanda ovos manter relativamente aquecida neste inicio novembro industrias continuam elevando compras producao fim ano oferta ovos menores permanece alta limitando novos reajustes precos segundo pesquisadores ovos maiores porem disponibilidade segue restrita</t>
+  </si>
+  <si>
+    <t>cotacoes trigo mercado lotes parana rio grande sul sao paulo registraram altas primeiro mes conforme dados elevacao atrelada baixa disponibilidade cereal boa qualidade retracao vendedores levantamentos mostram moinhos continuam grande interesse compra prevalecendo negociacoes pontuais pequenas quantidades muitas dessas empresas aguardam entrada maior volume trigo argentino proximos periodos lado vendedor produtores seguem focados colheita soja milho muitos acreditam novas valorizacoes grao devido dificuldade encontrar trigo boa qualidade tanto parana quanto rio grande sul valorizacao dolar torna trigo importado caro</t>
+  </si>
+  <si>
     <t>apesar bom ritmo exportacoes mes janeiro precos milho regioes portos voltaram recuar influenciados queda valores internacionais aquecimento negociacoes soja interior pais tambem havido pequena desvalorizacao campo avanca semeio cereal segunda safra parana mato grosso principais produtores janeiro precos paranagua acumularam queda regiao santos recuo campinas indicador esalqbmfbovespa apesar baixa regioes portos ritmo embarque intenso janeiro segundo secex janeiro dias uteis exportadas milhoes toneladas milho media diaria dias uteis mil toneladas</t>
   </si>
   <si>
+    <t>intensa queda precos mercado suinos iniciada semana passada manteve ultimos dias chegando menores valores desde outubro outro lado principais insumos utilizados atividade suinicola milho farelo soja valorizado desde comeco novembro reduzindo poder compra produtores independentes assim relacao troca suino vivo insumos nesta semana chegou menor patamar desde julho campinas sp relacao troca frente milho recuou desde inicio mes saindo quilos cereal quilo animal vivo proporcao ultima quintafeira chapeco sc queda relacao quilos milho quilo suino sao menores patamares desde primeira quinzena julho segundo pesquisadores alta insumos produtores passaram ofertar animais pois custos mantelos tempo granjas aumentaram dessa forma precos vivo carne enfraqueceram todas regioes pesquisadas</t>
+  </si>
+  <si>
+    <t>enquanto precos estao estaveis mercado internacional brasil desvalorizacao dolar frente real travado negociacoes enfraquecido precos internos ja distanciado valores ofertas compras vendas moeda norteamericana desvalorizou sete dias uteis consecutivos fechou r taxa comercial venda h sextafeira precos pedidos vendedores ofertas compradores chegaram ter diferenca tres reaissaca kg alem desvalorizacao dolar segundo colaboradores dividas custeio vencer proximos dias tendem elevar necessidade venda parte produtor pico colheita brasil deficit armazenagem escoamento tambem deve rapido marco indicador soja paranagua esalqbmfbovespa baseados negocios realizados queda r sc kg sextafeira media ponderada regioes paranaenses refletida indicador esalq caiu periodo indo r sc kg sextafeira menor valor dias uteis</t>
+  </si>
+  <si>
     <t>poder compra suinocultores menor neste inicio fevereiro devido altas precos milho principais insumos utilizados atividade junto farelo continuidade quedas cotacoes animal vivo acordo pesquisadores clima adverso altas cotacoes externas milho valorizacao dolar frente real elevado precos cereal forte desvalorizacao suino vivo mercado interno vez resultado recuo precos mercado atacadista decorrencia menor demanda frente farelo soja relacao troca tambem desfavoravel produtor neste caso pesou principalmente recuo cotacao animal vivo</t>
   </si>
   <si>
@@ -601,31 +808,109 @@
     <t>cotacoes carne frango apresentaram movimentos diferentes ultimos dias regioes pesquisadas algumas pracas feriado ultima sextafeira fez compras antecipadas influenciando leves reajustes precos ja demais pracas entrada salario conseguiu aquecer demanda segundo alguns colaboradores aumento preco carne frango correr agosto afastado parte consumidores desse produto relacao mercado frango vivo preco medio pago produtor segue estavel cotacoes principais insumos atividade farelo soja milho continuam pressionando rentabilidade avicultor</t>
   </si>
   <si>
+    <t>vendedores soja resistido propostas compradores baixa efetivacao negocios acordo informacoes muitos vendedores fizeram caixa momentos anteriores outros ainda estao cumprindo contratos pratica vendedores permanecem firmes ofertas enquanto compradores pressionam fundamentados quedas mercado externo tudo indica mercado spot baixa liquidez durante segundo semestre agentes voltados apenas nova safra culturas inverno quanto precos indicador esalqbmfbovespa produto transferido armazens porto paranagua recuou maio junho finalizando r saca kg convertido dolar moeda prevista contratos futuros bmfbovespa indicador esalqbmfbovespa fechou us sc kg sexta baixa periodo media ponderada regioes paranaenses refletida indicador esalq baixa maio junho indo r sc kg sextafeira</t>
+  </si>
+  <si>
+    <t>apesar bons estoques trigo mercado internacional fatores climaticos causado instabilidade cotacoes mercados fisico especialmente futuro estoques estao proximos media historica final temporada equivaliam consumo mundial contra media ultimos anos assim qualquer fator reduza oferta tende pressionalos aumentando disputa area segundo momento sobretudo soja milho cujos estoques estao niveis considerados baixos brasil segundo informacoes apreensao externa favoreceu ligeira melhora liquidez</t>
+  </si>
+  <si>
+    <t>precos frango vivo carne continuam registrando fortes altas mercado brasileiro ultimas semanas valores animal subiram todas regioes acompanhadas medias algumas pracas atingindo patamares recordes termos nominais considerada toda serie iniciada segundo colaboradores alto custo producao animal continua sendo principal motivo sucessivos reajustes nesse cenario avicultores conseguido recuperar parte poder compra frente principais insumos atividade milho farelo soja</t>
+  </si>
+  <si>
+    <t>segundo dados precos soja brasil continuaram firmes ultimos dias demanda prevalecendo sobre oferta compradores internacionais seguem ativos registros grandes quantidades serem embarcadas portos brasileiros principalmente santos paranagua proximos dias enquanto dados oferta vao sendo reajustados baixo dando suporte valores marco indicador esalqbmfbovespa produto transferido armazens porto paranagua subiu expressivos r saca kg sextafeira convertido dolar moeda prevista contratos futuros bmfbovespa indicador fechou us sc kg sexta aumento periodo media ponderada regioes paranaenses refletida indicador esalq elevacao marco indo r sc kg</t>
+  </si>
+  <si>
+    <t>movimento baixa precos suino vivo persiste todas regioes pesquisadas colaboradores atribuem comportamento fraca demanda carne suina varejo levantamentos segmentos produtor atacadista ainda nao identificam alteracao demanda decorrencia desoneracao impostos federais apesar dessas perdas insumos importantes atividade milho farelo soja apresentam desvalorizacoes ainda maiores proporcionando melhora poder compra suinocultores</t>
+  </si>
+  <si>
     <t>agentes brasileiros estao atentos avanco trabalhos campo desenvolvimento lavouras verao safra segundo pesquisadores ainda ha incertezas sobre tamanho safra verao assim atraso cultivo soja algumas regioes podera afetar semeio lavouras milho segunda safra periodo considerado ideal impactaria negativamente produtividade possibilidade chuvas cessarem cedo observado outro fator preocupacao relacao precos indicador esalqbmfbovespa representa negocios segmento lotes regiao campinas sp subiu novembro fechando r saca kg nessa segundafeira considerada taxa desconto npr regiao campinas preco medio vista r sc kg segunda alta periodo</t>
   </si>
   <si>
+    <t>consecutivas altas precos trigo grao sido repassadas farinhas acordo pesquisadores estimativas sobre safra mundial principalmente brasileira devem manter cotacoes patamares altos proximos meses concorrencia area trigo soja milho cenario mundial deve outro fator limitara quedas segundo pesquisadores recentes elevacoes cotacoes internas preocupado industrias paes massas biscoitos porque industrias nao esperavam alteracoes expressivas valores derivados trigo assim muitas unidades agora tentam fazer contratos enquanto nao ha novos reajustes tabelas contudo moinhos nao estao realizando contratos entrega farinha prazo superior dias devido instabilidade mercado materiaprima</t>
+  </si>
+  <si>
+    <t>cotacoes suino vivo carne continuam queda apesar oferta animais abate relativamente baixa demanda enfraquecida pressionado valores nessa quartafeira preco suino vivo fechou r kg regiao sp valor menor parcial mes atacado grande sao paulo carcaca especial suina acumula queda periodo r kg nessa quartafeira carcaca comum recuou negociada r kg segundo pesquisadores apesar quedas cotacoes carne animal baixas acumuladas valores milho farelo soja sido acentuadas aumentando poder compra suinocultores frente insumos neste inicio ano</t>
+  </si>
+  <si>
+    <t>menor demanda externa cautela compradores domesticos devido elevado frete rodoviario pressionaram cotacoes complexo soja brasil ultimos dias assim grande parte agentes prefere aguardar negociar proximas semanas visto tendencia reducao frete rodoviario devido finalizacao colheita milho retomada frete retorno diante importacoes insumos safra</t>
+  </si>
+  <si>
+    <t>movimento alta precos frango vivo mercado spot iniciado final maio segue firme nesta segunda quinzena junho ja precos principais insumos utilizados alimentacao animais milho farelo soja estao queda muitas regioes neste mes resultou forte melhora poder compra avicultores frente insumos parcial junho maio junho aumento cotacoes frango vivo expressivo praticamente todas regioes pesquisadas grande sao paulo media dessa quintafeira fechou r kg forte elevacao mes segundo colaboradores mercado avicola vinha tendo dificuldades repassar altos custos producao valores animais vivos maio reducao oferta estruturada players setor mercado voltou ficar enxuto junho conseguido repassar parte elevacao custos producao assim apesar inicio segunda quinzena geralmente demanda enfraquece mercado manteve equilibrado</t>
+  </si>
+  <si>
     <t>poder compra suinocultores frente milho principais insumos atividade subiu expressivamente neste mes segundo pesquisadores alem altas valores animal vivo cotacoes cereal vem caindo forca muitas regioes brasileiras pressionadas avanco colheita segunda safra ja quanto farelo soja poder compra cresceu algumas pracas diminuiu outras regiao sp braganca paulista campinas piracicaba sao paulo sorocaba poder compra suinocultor independente aumentou correr deste mes frente milho relacao farelo chapeco sc poder compra produtores aumentou frente milho caiu relacao farelo</t>
   </si>
   <si>
+    <t>embora precos trigo grao sigam queda grande parte regioes brasileiras reacoes rio grande sul ultima semana novas altas sao paulo refletindo boa liquidez leiloes conab estado gaucho valores primeira quinzena menores patamares desde fev modo geral demanda segue enfraquecida spot moinhos abastecidos processamento curto prazo segundo pesquisadores devido baixos precos ofertados compradores triticultores seguem retraidos apesar alguns sinalizarem intencao liberar espaco armazens recebimento soja milho safra verao</t>
+  </si>
+  <si>
+    <t>maioria regioes pesquisadas valores carne frango recuaram ultimos dias apesar preco vivo seguir estavel segundo pesquisadores expectativa setor consumo estaria aquecido devido inicio mes maior competitividade dessa proteina frente outras carnes nao concretizado alem disso atacadistas podem ter reduzido pontualmente margem lucro oferecido produto cotacoes menores justamente tentar incentivar demanda colaboradores relatam receio possiveis manifestacoes proximos dias prejudiquem transporte comercializacao animal carne bem abastecimento principais insumos utilizados atividade milho farelo soja</t>
+  </si>
+  <si>
+    <t>precos ovos recuaram nesta semana refletindo principalmente reducao demanda segundo agentes setor consultados compradores estao resistentes expectativa novas desvalorizacoes proximos dias alem disso baixas temperaturas favorecido armazenamento adequado ovos contribuindo aumento estoques assim pressionando valores entanto apesar desvalorizacoes relacao troca ovos principais insumos utilizados atividade milho farelo soja segue favoravel avicultor postura cujo poder compra neste mes ainda maior agosto ano passado</t>
+  </si>
+  <si>
     <t>cotacoes milho continuam subindo mercado interno devido retracao vendedores acreditam novas valorizacoes proximas semanas comportamento vez atrelado incertezas quanto desenvolvimento nova safra verao milho soja bom ritmo exportacoes nesse contexto segundo colaboradores vendedores vem postergando negociacoes grandes lotes limitando volumes ofertados compradores outro lado estao ativos mercado visto estao estoques reduzidos assim indicador esalqbmfbovespa campinassp subiu acumulado mes r saca quilos sextafeira</t>
   </si>
   <si>
+    <t>liquidez voltou diminuir mercado brasileiro milho segundo pesquisadores perspectivas diferentes quanto precos proximas semanas eou meses ampliaram diferenca valores regioes acompanhadas dificultando acordos compradores vendedores foco agentes continua exportacoes cultivo nova safra verao soja milho quanto precos segundo colaboradores oferta cereal continua restrita retracao compradores domesticos vinha pressionando cotacoes regiao campinas sp sextafeira especificamente compradores aumentar valor ofertas devido necessidade imediata adquirir lotes impulsionou indicador esalqbmfbovespa regiao paulista frente sexta anterior fechando r saca quilos dia</t>
+  </si>
+  <si>
     <t>cotacoes seguem firmes mercado ovos refletindo oferta restrita produto maioria regioes pesquisadas baixas temperaturas ultimos dias reduziram producao granjas algumas chegaram registrar queda producao ultimos sete dias alem disso conforme colaboradores demanda ovos aumentou nesse comeco mes apesar ferias escolares diminuem vendas destinadas merenda costumam alterar padroes consumo julho segundo agentes setor consultados ritmo comercializacao tambem segue bom favorecido baixos patamares precos principais insumos utilizados atividade milho farelo soja</t>
   </si>
   <si>
+    <t>cotacoes arroz casca registraram alta rio grande sul junho refletindo recuo orizicultores maior interesse industrias repor estoques especialmente segunda quinzena mes segundo pesquisadores produtores preferiram negociar outros produtos periodo soja lado comprador maior demanda industrias casca armazenado propriedades rurais principalmente segunda metade mes ja primeira quinzena chuvas frequentes dificultaram carregamento casca propriedades maior dificuldade acesso maio junho indicador esalqsenarrs graos inteiros subiu fechando r sc kg dia</t>
+  </si>
+  <si>
+    <t>industrias rio grande sul consultadas estao pouco ativas mercado processando arroz disponivel estoques produtores vez priorizado comercializacao soja quanto precos estao praticamente estaveis maio indicador esalqsenarrs graos inteiros subiu fechando r sc kg nessa tercafeira</t>
+  </si>
+  <si>
+    <t>proximidade intensificacao colheita segunda safra intervencoes governamentais dolar forte real voltaram aquecer negociacoes milho exportacao portos brasileiros alem disso segundo pesquisadores demanda domestica enfraquecida parte expressiva armazens ainda comprometida soja maio embarques cereal brasileiro somaram mil toneladas alta relacao abril segundo secex quanto precos mercado brasileiro estao queda devido maior oferta cereal campinas sp pressao compradora continua vendedores comportamento flexivel favorecendo realizacao negocios nesse cenario indicador esalqbmfbovespa caiu maio junho fechando r saca quilos sextafeira</t>
+  </si>
+  <si>
     <t>valorizacao dolar ultima semana produtores voltaram afastar mercado cenario elevou precos soja grao boa parte producao temporada ja comprometida vendedores voltam atencoes cultivo nova safra alem disso pesquisadores indicam demandas interna principalmente producao biodiesel externa seguem aquecidas sul brasil precipitacoes ultima semana menos intensas produtores conseguiram avancar trabalhos campo centrooeste onde clima seco precipitacoes algumas regioes previsoes chuvas outras animaram sojicultores iniciarem eou avancarem cultivo oleaginosa</t>
   </si>
   <si>
+    <t>menor demanda interna carne frango devido renda limitada populacao sobretudo inicio deste mes pressionou valor medio animal vivo mercado independente maio junho conforme indicam pesquisas quanto principais insumos atividade milho farelo soja cenario tambem desvalorizacao nesse periodo movimento queda ocorreu forma menos intensa diante disso poder compra avicultores corte frente insumos vem recuando junho apos terem avancado tres meses seguidos fonte</t>
+  </si>
+  <si>
+    <t>quedas precos principais insumos utilizados avicultura postura milho farelo soja dado certo alivio produtores voltaram enfrentar recuo cotacoes ovos desde final ultima semana pesquisadores indicam embora oferta ovos nao considerada elevada decorrencia avanco descartes retracao demanda pressionou cotacoes expectativa colaboradores proximidade inicio mes tradicionais festas juninas possam estimular vendas curto prazo</t>
+  </si>
+  <si>
     <t>iniciadas meados marco quedas precos suino vivo estao intensas observadas principais insumos utilizados atividade milho farelo soja cenario vem reduzindo poder compra produtores suinos comparandose parcial abril periodo ano passado mercado carne suina movimento tambem recuo precos conta justamente menores consumos interno externo segundo colaboradores desajuste oferta demanda vem principalmente sul pais acaba enviando produto outros estados reforcando pressao sobre valores estoques nao aumentem expressivamente industrias vem operando cotacoes baixas promocoes aumento prazos pagamento</t>
   </si>
   <si>
+    <t>mercado milho ainda busca direcao geral ainda prevalecem movimentos distintos precos pracas produtoras comercializacao acompanhadas avanco colheita milho primeira safra sul sudeste brasil elevado oferta grao mercado nacional pressionado valores algumas pracas outro lado retracao parte vendedores prefere negociar soja continua sustentando cotacoes outras regioes nessa tercafeira indicador esalqbmfbovespa referente regiao campinas sp fechou r saca kg recuo frente terca anterior considerados negocios tambem campinas cujos prazos pagamento sao descontados taxa desconto npr preco medio vista r sc recuo periodo</t>
+  </si>
+  <si>
+    <t>mercado fisico brasileiro perspectiva aumento exportacoes estimula reajustes contratos antecipados principalmente daqueles entrega segundo semestre segundo pesquisadores contexto reforca postura retraida vendedores spot priorizam comercializacao soja frustram compradores mostram interessados abastecer estoques assim cenario proporcionado sustentacao milho diante dados oferta demanda sinalizariam expressivo excedente interno indicador esalqbmfbovespa referente regiao campinas sp fechou nessa tercafeira r sc queda sete dias alta leve mes considerados negocios tambem campinas cujos prazos pagamento sao descontados taxa desconto npr preco medio vista r sc dia queda sete dias alta mes</t>
+  </si>
+  <si>
+    <t>negociacoes mercado trigo grao enfraqueceram ultimos dias porem precos mantem firmes segundo pesquisadores muitos moinhos estao apenas recebendo grao negociado anteriormente produtores permanecem voltados safra verao alem acreditam alta dolar possa valorizar cereal proximos meses completar paralisacao caminhoneiros comprometido entrega grao ultimos dias rio grande sul oferta trigo pouco maior parana devido necessidade liberacao espaco silos soja porem estado gaucho serios problemas climaticos durante desenvolvimento cultura boa parte producao ficou valor comercial moinhos mercado brasileiro sendo destinada exportacao paises africanos asiaticos racao animal cenario tambem eleva necessidade importacao cereal atender demanda nacional grao estimada conab milhoes t volume maior safra anterior</t>
+  </si>
+  <si>
     <t>comercializacao trigo grao aquecida ultima semana relacao anteriores segundo pesquisadores moinhos ativos reposicao estoques dado preferencia cereal nacional constante valorizacao dolar trigo importado cada caro compradores brasileiros produtores vez tambem demonstraram maior interesse negociacoes produto estocado objetivo fazer caixa ja valores atuais sao considerados atrativos cenario fortalecido precos trigo pode influenciar decisao plantio cereal detrimento milho segunda safra temporada esperase avanco area plantada principalmente norte parana razao tambem atraso cultivo soja pode ficar janela ideal porem ainda nao possivel mensurar impacto sobre area total estado</t>
   </si>
   <si>
     <t>aumento precos milho segue pressionando poder compra suinocultores nesta primeira quinzena registrou pior marca mes marco toda serie suinos iniciouse relacao farelo soja apesar valores desse insumo estarem queda desde final janeiro poder compra suinocultor primeira quinzena marco tambem menor ha ano segundo pesquisadores quedas precos suino vivo seguem atreladas aumento oferta ultimos meses insumos utilizados alimentacao caros produtores antecipam terminacao animal ofertam abaixo peso ideal aumentando disponibilidade animais abate</t>
   </si>
   <si>
+    <t>precos soja derivados cairam brasil ultimos dias consequencia avanco colheita ja eleva disponibilidade grao mercado interno entanto quedas limitadas cambio aqueceu interesse vendedor negociacoes so nao intensas conta periodo carnaval paralisou mercado alguns dias semana passada campo sojicultores algumas regioes centrooeste estao preocupados clima chuvoso pode atrasar colheita prejudicar qualidade grao outro lado chuvas beneficiam lavouras ainda desenvolvimento vale ressaltar mato grosso ha grande diferenca desenvolvimento lavoura outra mato grosso sul colheita segue bom ritmo produtores esperam boa safra parana chuvas interromperam colheita ultimos dias sojicultores ja voltaram trabalhos campos sinalizam produtividade dentro esperado</t>
+  </si>
+  <si>
+    <t>precos domesticos suino vivo carne seguem queda influenciados ampla oferta valores milho farelo soja bastante elevados suinocultores aumentado abates tentativa economizar alimentacao manter margens maior volume exportado carne suina in natura janeiro suficiente estancar quedas mercado nacional mes passado exportadas mil toneladas carne suina in natura dezembro expressivos acima embarques janeiro apesar atipico periodo alta esperada alguns agentes setor funcao dolar valorizado janeiro receita r milhoes recorde periodo maior jan dolar faturamento us milhoes aumento sobre periodo ano passado</t>
+  </si>
+  <si>
     <t>movimento alta precos ovos ganhou forca segunda quinzena mes impulsionado principalmente menor oferta domestica alem descartes ja programados poedeiras elevados valores insumos utilizados avicultura postura milho farelo soja feito produtores reduzam quantidade aves alojadas assim volume alimento disponibilizado cenario reforca reducao volume produzido consequentemente aumentos cotacoes demanda tambem segue relativamente aquecida contribuindo impulsionar valores</t>
+  </si>
+  <si>
+    <t>maior demanda festas fim ano comecou surtir efeito mercado ovos ultima semana precos subindo ate bastos sp principal regiao produtora acompanhada segundo pesquisadores valorizacoes ajudam partes manter rentabilidade avicultores postura embora valores principais insumos utilizados atividade milho farelo soja sigam elevados</t>
+  </si>
+  <si>
+    <t>cotacoes suino vivo voltaram reagir maioria pracas pesquisadas ultimos dias apesar disso animal vivo ainda desvalorizado relacao periodo outro lado cotacoes principais insumos utilizados atividade milho farelo soja registram alta comparativo anual conforme indicam dados resultado poder compra suinocultores independentes paulistas catarinenses frente insumos menor vale lembrar produtores tambem enfrentam aumento itens participam custos fixos energia eletrica mao obra</t>
+  </si>
+  <si>
+    <t>volume chuva reduziu ultimos dias colheita soja intensificada atividades ja entrando reta final mato grosso principal produtor nacional oleaginosa acordo conab ate dia brasil colheu milhoes toneladas previstas temporada mato grosso percentual chegou segundo agentes mercado consultados produtividade qualidade safra estao excelentes maior parte pais reforca estimativas colheita recorde fonte</t>
   </si>
   <si>
     <t>Neutra</t>
@@ -986,7 +1271,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1025,29 +1310,26 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
-        <v>61</v>
-      </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>147</v>
       </c>
       <c r="D2" t="s">
-        <v>152</v>
+        <v>223</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>299</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G2">
-        <v>1.920307041095327E-30</v>
+        <v>0.9999994453240053</v>
       </c>
       <c r="H2">
-        <v>0.001360503492162663</v>
+        <v>4.50114974104498E-09</v>
       </c>
       <c r="I2">
-        <v>0.9986391478318023</v>
+        <v>4.503579424544192E-09</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1055,28 +1337,28 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="C3" t="s">
-        <v>101</v>
+        <v>148</v>
       </c>
       <c r="D3" t="s">
-        <v>153</v>
+        <v>224</v>
       </c>
       <c r="E3" t="s">
-        <v>204</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G3">
-        <v>9.270989215748456E-34</v>
+        <v>2.429397519499865E-20</v>
       </c>
       <c r="H3">
-        <v>0.975372193164305</v>
+        <v>0.000195464352043527</v>
       </c>
       <c r="I3">
-        <v>0.02462564346458275</v>
+        <v>0.9998045356475747</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1084,28 +1366,28 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>149</v>
       </c>
       <c r="D4" t="s">
-        <v>154</v>
+        <v>225</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>299</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
       </c>
       <c r="G4">
-        <v>5.8546000380346E-27</v>
+        <v>2.966034836231091E-12</v>
       </c>
       <c r="H4">
-        <v>0.9999996638704826</v>
+        <v>0.9997530364668555</v>
       </c>
       <c r="I4">
-        <v>3.361026533106808E-07</v>
+        <v>0.0002375762177545786</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1113,28 +1395,28 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>150</v>
       </c>
       <c r="D5" t="s">
-        <v>155</v>
+        <v>226</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G5">
-        <v>1.839986036171189E-36</v>
+        <v>1</v>
       </c>
       <c r="H5">
-        <v>0.9982886690042333</v>
+        <v>1.909939857889975E-38</v>
       </c>
       <c r="I5">
-        <v>0.001711128117190879</v>
+        <v>2.830832109732334E-27</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1142,28 +1424,28 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
+        <v>151</v>
       </c>
       <c r="D6" t="s">
-        <v>156</v>
+        <v>227</v>
       </c>
       <c r="E6" t="s">
+        <v>299</v>
+      </c>
+      <c r="F6" t="s">
         <v>8</v>
       </c>
-      <c r="F6" t="s">
-        <v>7</v>
-      </c>
       <c r="G6">
-        <v>1.512615277769809E-30</v>
+        <v>1.911904787879075E-09</v>
       </c>
       <c r="H6">
-        <v>0.5114066252540256</v>
+        <v>0.0003785589814537125</v>
       </c>
       <c r="I6">
-        <v>0.4885109207795175</v>
+        <v>0.9993967157062824</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1171,54 +1453,57 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
-        <v>105</v>
+        <v>152</v>
       </c>
       <c r="D7" t="s">
-        <v>157</v>
+        <v>228</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F7" t="s">
         <v>8</v>
       </c>
       <c r="G7">
-        <v>3.291091460775608E-13</v>
+        <v>1.13942536860805E-09</v>
       </c>
       <c r="H7">
-        <v>0.1957594614717951</v>
+        <v>0.02643708572532487</v>
       </c>
       <c r="I7">
-        <v>0.8042208883393008</v>
+        <v>0.9636758927051748</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>15</v>
       </c>
+      <c r="B8" t="s">
+        <v>89</v>
+      </c>
       <c r="C8" t="s">
-        <v>106</v>
+        <v>153</v>
       </c>
       <c r="D8" t="s">
-        <v>158</v>
+        <v>229</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G8">
-        <v>4.520633585340389E-28</v>
+        <v>0.9999999999837428</v>
       </c>
       <c r="H8">
-        <v>0.9990569109404926</v>
+        <v>3.45194219586279E-13</v>
       </c>
       <c r="I8">
-        <v>0.0009430834701184824</v>
+        <v>1.683617274495058E-16</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1226,13 +1511,13 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="C9" t="s">
-        <v>107</v>
+        <v>154</v>
       </c>
       <c r="D9" t="s">
-        <v>159</v>
+        <v>230</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
@@ -1241,42 +1526,39 @@
         <v>7</v>
       </c>
       <c r="G9">
-        <v>9.929405987526896E-29</v>
+        <v>2.478415263674297E-13</v>
       </c>
       <c r="H9">
-        <v>0.9628016633694074</v>
+        <v>0.8230656768934073</v>
       </c>
       <c r="I9">
-        <v>0.03718446899674366</v>
+        <v>0.02144367669804665</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
-        <v>68</v>
-      </c>
       <c r="C10" t="s">
-        <v>108</v>
+        <v>155</v>
       </c>
       <c r="D10" t="s">
-        <v>160</v>
+        <v>231</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G10">
-        <v>2.590448805810276E-23</v>
+        <v>0.999874831300001</v>
       </c>
       <c r="H10">
-        <v>0.5148782097534655</v>
+        <v>0.0001039614183269957</v>
       </c>
       <c r="I10">
-        <v>0.4848836271030626</v>
+        <v>2.120728165431831E-05</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1284,25 +1566,25 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>109</v>
+        <v>156</v>
       </c>
       <c r="D11" t="s">
-        <v>161</v>
+        <v>232</v>
       </c>
       <c r="E11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F11" t="s">
         <v>7</v>
       </c>
       <c r="G11">
-        <v>1.109149184360774E-28</v>
+        <v>0.01913146500578146</v>
       </c>
       <c r="H11">
-        <v>0.9745178693208086</v>
+        <v>0.9480449405118038</v>
       </c>
       <c r="I11">
-        <v>0.02547989098119209</v>
+        <v>0.03282355312821794</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1310,28 +1592,28 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="C12" t="s">
-        <v>110</v>
+        <v>157</v>
       </c>
       <c r="D12" t="s">
-        <v>162</v>
+        <v>233</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" t="s">
         <v>7</v>
       </c>
       <c r="G12">
-        <v>1.064543338690142E-33</v>
+        <v>1.201993934812911E-26</v>
       </c>
       <c r="H12">
-        <v>0.999964376631324</v>
+        <v>0.9992015007794109</v>
       </c>
       <c r="I12">
-        <v>3.5623368658406E-05</v>
+        <v>0.0007984819474617441</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1339,10 +1621,10 @@
         <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>111</v>
+        <v>158</v>
       </c>
       <c r="D13" t="s">
-        <v>163</v>
+        <v>234</v>
       </c>
       <c r="E13" t="s">
         <v>7</v>
@@ -1351,24 +1633,27 @@
         <v>7</v>
       </c>
       <c r="G13">
-        <v>5.69949201463441E-23</v>
+        <v>8.510814355583542E-11</v>
       </c>
       <c r="H13">
-        <v>0.9997951323059763</v>
+        <v>0.9971144083597385</v>
       </c>
       <c r="I13">
-        <v>0.0002048670992037835</v>
+        <v>0.002723286287826522</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>21</v>
       </c>
+      <c r="B14" t="s">
+        <v>92</v>
+      </c>
       <c r="C14" t="s">
-        <v>112</v>
+        <v>159</v>
       </c>
       <c r="D14" t="s">
-        <v>164</v>
+        <v>235</v>
       </c>
       <c r="E14" t="s">
         <v>8</v>
@@ -1377,13 +1662,13 @@
         <v>8</v>
       </c>
       <c r="G14">
-        <v>4.989372990124677E-41</v>
+        <v>1.747103489721654E-23</v>
       </c>
       <c r="H14">
-        <v>0.0002689168714831968</v>
+        <v>0.0002289934953560722</v>
       </c>
       <c r="I14">
-        <v>0.9997310831285415</v>
+        <v>0.9997694891199318</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1391,25 +1676,25 @@
         <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>113</v>
+        <v>160</v>
       </c>
       <c r="D15" t="s">
-        <v>165</v>
+        <v>236</v>
       </c>
       <c r="E15" t="s">
-        <v>204</v>
+        <v>6</v>
       </c>
       <c r="F15" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G15">
-        <v>9.068088822376561E-29</v>
+        <v>0.9999978288579122</v>
       </c>
       <c r="H15">
-        <v>0.1607874295312411</v>
+        <v>1.972862918062007E-06</v>
       </c>
       <c r="I15">
-        <v>0.8392118195031668</v>
+        <v>1.982791733849582E-07</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1417,28 +1702,28 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="C16" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="D16" t="s">
-        <v>166</v>
+        <v>237</v>
       </c>
       <c r="E16" t="s">
-        <v>8</v>
+        <v>299</v>
       </c>
       <c r="F16" t="s">
         <v>8</v>
       </c>
       <c r="G16">
-        <v>1.381966499241037E-14</v>
+        <v>9.595876786493686E-07</v>
       </c>
       <c r="H16">
-        <v>0.0002582737264466738</v>
+        <v>0.001166902161780329</v>
       </c>
       <c r="I16">
-        <v>0.975678903288998</v>
+        <v>0.9814642638042861</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1446,28 +1731,28 @@
         <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="C17" t="s">
-        <v>115</v>
+        <v>162</v>
       </c>
       <c r="D17" t="s">
-        <v>167</v>
+        <v>238</v>
       </c>
       <c r="E17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F17" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G17">
-        <v>1.32770925092348E-13</v>
+        <v>1.564522024359873E-06</v>
       </c>
       <c r="H17">
-        <v>0.9977902413692447</v>
+        <v>3.253591664206019E-05</v>
       </c>
       <c r="I17">
-        <v>0.002209327437368353</v>
+        <v>0.9924541672056998</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1475,28 +1760,28 @@
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="C18" t="s">
-        <v>116</v>
+        <v>163</v>
       </c>
       <c r="D18" t="s">
-        <v>168</v>
+        <v>239</v>
       </c>
       <c r="E18" t="s">
         <v>7</v>
       </c>
       <c r="F18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G18">
-        <v>1.32289406115119E-17</v>
+        <v>0.9999744173840315</v>
       </c>
       <c r="H18">
-        <v>0.9638013375084351</v>
+        <v>5.373019601350014E-06</v>
       </c>
       <c r="I18">
-        <v>0.01117685562332354</v>
+        <v>2.020911479841508E-05</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1504,28 +1789,28 @@
         <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="C19" t="s">
-        <v>117</v>
+        <v>164</v>
       </c>
       <c r="D19" t="s">
-        <v>169</v>
+        <v>240</v>
       </c>
       <c r="E19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G19">
-        <v>2.185227290685188E-18</v>
+        <v>0.1588106171867049</v>
       </c>
       <c r="H19">
-        <v>0.9909209152085603</v>
+        <v>4.923942524726873E-06</v>
       </c>
       <c r="I19">
-        <v>0.008741835302493554</v>
+        <v>0.8411794677095958</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1533,28 +1818,28 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="C20" t="s">
-        <v>118</v>
+        <v>165</v>
       </c>
       <c r="D20" t="s">
-        <v>170</v>
+        <v>241</v>
       </c>
       <c r="E20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F20" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G20">
-        <v>2.547518977907011E-25</v>
+        <v>8.780138154162716E-07</v>
       </c>
       <c r="H20">
-        <v>0.991608454012611</v>
+        <v>0.0004297829458850179</v>
       </c>
       <c r="I20">
-        <v>0.008385795284703873</v>
+        <v>0.9995693376053952</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1562,54 +1847,57 @@
         <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="C21" t="s">
-        <v>119</v>
+        <v>166</v>
       </c>
       <c r="D21" t="s">
-        <v>171</v>
+        <v>242</v>
       </c>
       <c r="E21" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F21" t="s">
-        <v>8</v>
+        <v>299</v>
       </c>
       <c r="G21">
-        <v>3.180836265249022E-10</v>
+        <v>8.22279462079521E-07</v>
       </c>
       <c r="H21">
-        <v>1.06172320866831E-07</v>
+        <v>0.003944673411594979</v>
       </c>
       <c r="I21">
-        <v>0.9983293468877349</v>
+        <v>0.03445870853071474</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>29</v>
       </c>
+      <c r="B22" t="s">
+        <v>99</v>
+      </c>
       <c r="C22" t="s">
-        <v>120</v>
+        <v>167</v>
       </c>
       <c r="D22" t="s">
-        <v>172</v>
+        <v>243</v>
       </c>
       <c r="E22" t="s">
         <v>7</v>
       </c>
       <c r="F22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G22">
-        <v>3.758568846965364E-13</v>
+        <v>0.9992010170888157</v>
       </c>
       <c r="H22">
-        <v>0.6152117126731333</v>
+        <v>0.0007989286317439618</v>
       </c>
       <c r="I22">
-        <v>0.05003826393473887</v>
+        <v>5.427936855418423E-08</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1617,28 +1905,28 @@
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="C23" t="s">
-        <v>121</v>
+        <v>168</v>
       </c>
       <c r="D23" t="s">
-        <v>173</v>
+        <v>244</v>
       </c>
       <c r="E23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" t="s">
         <v>8</v>
       </c>
-      <c r="F23" t="s">
-        <v>7</v>
-      </c>
       <c r="G23">
-        <v>2.425225604113184E-19</v>
+        <v>7.435720929755678E-20</v>
       </c>
       <c r="H23">
-        <v>0.9804941366325033</v>
+        <v>0.1113462138514875</v>
       </c>
       <c r="I23">
-        <v>0.01950246122762686</v>
+        <v>0.8886537642134402</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1646,25 +1934,25 @@
         <v>31</v>
       </c>
       <c r="C24" t="s">
-        <v>122</v>
+        <v>169</v>
       </c>
       <c r="D24" t="s">
-        <v>174</v>
+        <v>245</v>
       </c>
       <c r="E24" t="s">
-        <v>204</v>
+        <v>8</v>
       </c>
       <c r="F24" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G24">
-        <v>1.769227718039001E-17</v>
+        <v>0.9785559054758179</v>
       </c>
       <c r="H24">
-        <v>0.01935232343539397</v>
+        <v>0.0007791091040362557</v>
       </c>
       <c r="I24">
-        <v>0.9139083058678821</v>
+        <v>0.02066498078701482</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1672,39 +1960,42 @@
         <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="C25" t="s">
-        <v>123</v>
+        <v>170</v>
       </c>
       <c r="D25" t="s">
-        <v>175</v>
+        <v>246</v>
       </c>
       <c r="E25" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F25" t="s">
         <v>7</v>
       </c>
       <c r="G25">
-        <v>1.751514554748892E-16</v>
+        <v>1.624565470733125E-06</v>
       </c>
       <c r="H25">
-        <v>0.9999796301671502</v>
+        <v>0.994493845875481</v>
       </c>
       <c r="I25">
-        <v>1.942902406533695E-05</v>
+        <v>0.0003139094385176898</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>33</v>
       </c>
+      <c r="B26" t="s">
+        <v>102</v>
+      </c>
       <c r="C26" t="s">
-        <v>124</v>
+        <v>171</v>
       </c>
       <c r="D26" t="s">
-        <v>176</v>
+        <v>247</v>
       </c>
       <c r="E26" t="s">
         <v>7</v>
@@ -1713,13 +2004,13 @@
         <v>8</v>
       </c>
       <c r="G26">
-        <v>5.216975998794412E-14</v>
+        <v>2.170895922007902E-09</v>
       </c>
       <c r="H26">
-        <v>0.005627330457088272</v>
+        <v>0.06757283709545261</v>
       </c>
       <c r="I26">
-        <v>0.9943722551508755</v>
+        <v>0.929890850314852</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1727,13 +2018,13 @@
         <v>34</v>
       </c>
       <c r="B27" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="C27" t="s">
-        <v>125</v>
+        <v>172</v>
       </c>
       <c r="D27" t="s">
-        <v>177</v>
+        <v>248</v>
       </c>
       <c r="E27" t="s">
         <v>7</v>
@@ -1742,39 +2033,42 @@
         <v>7</v>
       </c>
       <c r="G27">
-        <v>4.34706584849479E-20</v>
+        <v>1.425330984696872E-24</v>
       </c>
       <c r="H27">
-        <v>0.9580401191267797</v>
+        <v>0.5179239462410783</v>
       </c>
       <c r="I27">
-        <v>0.04195980287410397</v>
+        <v>0.4820760533649421</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>35</v>
       </c>
+      <c r="B28" t="s">
+        <v>104</v>
+      </c>
       <c r="C28" t="s">
-        <v>126</v>
+        <v>173</v>
       </c>
       <c r="D28" t="s">
-        <v>178</v>
+        <v>249</v>
       </c>
       <c r="E28" t="s">
-        <v>204</v>
+        <v>7</v>
       </c>
       <c r="F28" t="s">
         <v>7</v>
       </c>
       <c r="G28">
-        <v>4.175790738902128E-16</v>
+        <v>1.540667036516456E-15</v>
       </c>
       <c r="H28">
-        <v>0.5748055841161707</v>
+        <v>0.8324634332039166</v>
       </c>
       <c r="I28">
-        <v>0.04724431199719074</v>
+        <v>0.1135935828473825</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1782,28 +2076,28 @@
         <v>36</v>
       </c>
       <c r="B29" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="C29" t="s">
-        <v>127</v>
+        <v>174</v>
       </c>
       <c r="D29" t="s">
-        <v>179</v>
+        <v>250</v>
       </c>
       <c r="E29" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F29" t="s">
         <v>8</v>
       </c>
       <c r="G29">
-        <v>4.402162083720216E-23</v>
+        <v>1.163201456380646E-06</v>
       </c>
       <c r="H29">
-        <v>0.007720341031902857</v>
+        <v>3.003632733134733E-05</v>
       </c>
       <c r="I29">
-        <v>0.9922794238723696</v>
+        <v>0.9999445326308953</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1811,28 +2105,28 @@
         <v>37</v>
       </c>
       <c r="B30" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="C30" t="s">
-        <v>128</v>
+        <v>175</v>
       </c>
       <c r="D30" t="s">
-        <v>180</v>
+        <v>251</v>
       </c>
       <c r="E30" t="s">
-        <v>204</v>
+        <v>299</v>
       </c>
       <c r="F30" t="s">
-        <v>7</v>
+        <v>299</v>
       </c>
       <c r="G30">
-        <v>1.891412026081356E-23</v>
+        <v>1.599570478486785E-13</v>
       </c>
       <c r="H30">
-        <v>0.9185173174774458</v>
+        <v>1.168613488097773E-05</v>
       </c>
       <c r="I30">
-        <v>0.08148196439162535</v>
+        <v>2.179997113963383E-05</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1840,28 +2134,28 @@
         <v>38</v>
       </c>
       <c r="B31" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="C31" t="s">
-        <v>129</v>
+        <v>176</v>
       </c>
       <c r="D31" t="s">
-        <v>181</v>
+        <v>252</v>
       </c>
       <c r="E31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F31" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G31">
-        <v>1.724855199057E-18</v>
+        <v>0.000924136817513794</v>
       </c>
       <c r="H31">
-        <v>0.834625953393045</v>
+        <v>0.2673774807535489</v>
       </c>
       <c r="I31">
-        <v>0.1653740244890024</v>
+        <v>0.7302492071821984</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1869,54 +2163,57 @@
         <v>39</v>
       </c>
       <c r="B32" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="C32" t="s">
-        <v>130</v>
+        <v>177</v>
       </c>
       <c r="D32" t="s">
-        <v>182</v>
+        <v>253</v>
       </c>
       <c r="E32" t="s">
         <v>7</v>
       </c>
       <c r="F32" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G32">
-        <v>2.823869158332613E-23</v>
+        <v>9.884535704740671E-06</v>
       </c>
       <c r="H32">
-        <v>0.9985239004417648</v>
+        <v>0.006630122662419545</v>
       </c>
       <c r="I32">
-        <v>0.001424980494991465</v>
+        <v>0.9933598873805308</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
         <v>40</v>
       </c>
+      <c r="B33" t="s">
+        <v>109</v>
+      </c>
       <c r="C33" t="s">
-        <v>131</v>
+        <v>178</v>
       </c>
       <c r="D33" t="s">
-        <v>183</v>
+        <v>254</v>
       </c>
       <c r="E33" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F33" t="s">
         <v>7</v>
       </c>
       <c r="G33">
-        <v>4.482599446991652E-13</v>
+        <v>0.3319957848845271</v>
       </c>
       <c r="H33">
-        <v>0.9999347904763507</v>
+        <v>0.6679903659011512</v>
       </c>
       <c r="I33">
-        <v>5.632679548360335E-05</v>
+        <v>1.384910568172002E-05</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1924,28 +2221,28 @@
         <v>41</v>
       </c>
       <c r="B34" t="s">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="C34" t="s">
-        <v>132</v>
+        <v>179</v>
       </c>
       <c r="D34" t="s">
-        <v>184</v>
+        <v>255</v>
       </c>
       <c r="E34" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F34" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G34">
-        <v>6.427993058135988E-24</v>
+        <v>0.999952220610679</v>
       </c>
       <c r="H34">
-        <v>0.008673277605052692</v>
+        <v>4.591481348821422E-05</v>
       </c>
       <c r="I34">
-        <v>0.9912929846554275</v>
+        <v>1.864524970747026E-06</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1953,28 +2250,28 @@
         <v>42</v>
       </c>
       <c r="B35" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="C35" t="s">
-        <v>133</v>
+        <v>180</v>
       </c>
       <c r="D35" t="s">
-        <v>185</v>
+        <v>256</v>
       </c>
       <c r="E35" t="s">
-        <v>204</v>
+        <v>6</v>
       </c>
       <c r="F35" t="s">
-        <v>204</v>
+        <v>6</v>
       </c>
       <c r="G35">
-        <v>4.626020794505307E-08</v>
+        <v>0.8050107779481862</v>
       </c>
       <c r="H35">
-        <v>0.05951380758890493</v>
+        <v>0.001971533991379431</v>
       </c>
       <c r="I35">
-        <v>0.001920233604505345</v>
+        <v>0.02371683675190586</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1982,28 +2279,28 @@
         <v>43</v>
       </c>
       <c r="B36" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="C36" t="s">
-        <v>134</v>
+        <v>181</v>
       </c>
       <c r="D36" t="s">
-        <v>186</v>
+        <v>257</v>
       </c>
       <c r="E36" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F36" t="s">
         <v>7</v>
       </c>
       <c r="G36">
-        <v>1.033543004650933E-17</v>
+        <v>2.98357079651138E-16</v>
       </c>
       <c r="H36">
-        <v>0.9984523991638544</v>
+        <v>0.9962346942108219</v>
       </c>
       <c r="I36">
-        <v>0.00148626132221829</v>
+        <v>0.003764873183232898</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -2011,86 +2308,80 @@
         <v>44</v>
       </c>
       <c r="B37" t="s">
-        <v>85</v>
+        <v>113</v>
       </c>
       <c r="C37" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="D37" t="s">
-        <v>187</v>
+        <v>258</v>
       </c>
       <c r="E37" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G37">
-        <v>1.531735938389253E-21</v>
+        <v>0.0004740215099933085</v>
       </c>
       <c r="H37">
-        <v>0.1459285575253153</v>
+        <v>0.9995259784878494</v>
       </c>
       <c r="I37">
-        <v>0.8538077262546052</v>
+        <v>2.186784573765703E-12</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" t="s">
         <v>45</v>
       </c>
-      <c r="B38" t="s">
-        <v>86</v>
-      </c>
       <c r="C38" t="s">
-        <v>136</v>
+        <v>183</v>
       </c>
       <c r="D38" t="s">
-        <v>188</v>
+        <v>259</v>
       </c>
       <c r="E38" t="s">
-        <v>204</v>
+        <v>7</v>
       </c>
       <c r="F38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G38">
-        <v>8.750406496212061E-16</v>
+        <v>7.861216539959008E-29</v>
       </c>
       <c r="H38">
-        <v>0.003562761614073397</v>
+        <v>0.999614694032946</v>
       </c>
       <c r="I38">
-        <v>0.9963669357974614</v>
+        <v>0.0003853059627469384</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
         <v>46</v>
       </c>
-      <c r="B39" t="s">
-        <v>87</v>
-      </c>
       <c r="C39" t="s">
-        <v>137</v>
+        <v>184</v>
       </c>
       <c r="D39" t="s">
-        <v>189</v>
+        <v>260</v>
       </c>
       <c r="E39" t="s">
-        <v>7</v>
+        <v>299</v>
       </c>
       <c r="F39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G39">
-        <v>2.366648534961495E-20</v>
+        <v>4.22416051034456E-06</v>
       </c>
       <c r="H39">
-        <v>0.08856800470924177</v>
+        <v>0.999995771982085</v>
       </c>
       <c r="I39">
-        <v>0.9114311533820678</v>
+        <v>3.857414379411335E-09</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -2098,54 +2389,57 @@
         <v>47</v>
       </c>
       <c r="B40" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="C40" t="s">
-        <v>138</v>
+        <v>185</v>
       </c>
       <c r="D40" t="s">
-        <v>190</v>
+        <v>261</v>
       </c>
       <c r="E40" t="s">
         <v>8</v>
       </c>
       <c r="F40" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G40">
-        <v>7.447992365834099E-24</v>
+        <v>1.108339701973431E-38</v>
       </c>
       <c r="H40">
-        <v>0.9999785566964553</v>
+        <v>0.0005920338353041112</v>
       </c>
       <c r="I40">
-        <v>2.134190284182228E-05</v>
+        <v>0.9994079661619115</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
         <v>48</v>
       </c>
+      <c r="B41" t="s">
+        <v>115</v>
+      </c>
       <c r="C41" t="s">
-        <v>139</v>
+        <v>186</v>
       </c>
       <c r="D41" t="s">
-        <v>191</v>
+        <v>262</v>
       </c>
       <c r="E41" t="s">
-        <v>204</v>
+        <v>299</v>
       </c>
       <c r="F41" t="s">
-        <v>7</v>
+        <v>299</v>
       </c>
       <c r="G41">
-        <v>7.174366629828457E-27</v>
+        <v>7.998548695869229E-12</v>
       </c>
       <c r="H41">
-        <v>0.9999994873805526</v>
+        <v>0.07148859531353868</v>
       </c>
       <c r="I41">
-        <v>5.124999136204462E-07</v>
+        <v>1.841111686047717E-06</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -2153,28 +2447,28 @@
         <v>49</v>
       </c>
       <c r="B42" t="s">
-        <v>89</v>
+        <v>116</v>
       </c>
       <c r="C42" t="s">
-        <v>140</v>
+        <v>187</v>
       </c>
       <c r="D42" t="s">
-        <v>192</v>
+        <v>263</v>
       </c>
       <c r="E42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F42" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G42">
-        <v>2.071717659299359E-37</v>
+        <v>0.9915491029292123</v>
       </c>
       <c r="H42">
-        <v>9.573262482941628E-06</v>
+        <v>0.007045093620572413</v>
       </c>
       <c r="I42">
-        <v>0.9999904233890622</v>
+        <v>0.001405799578247854</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -2182,28 +2476,28 @@
         <v>50</v>
       </c>
       <c r="B43" t="s">
-        <v>90</v>
+        <v>117</v>
       </c>
       <c r="C43" t="s">
-        <v>141</v>
+        <v>188</v>
       </c>
       <c r="D43" t="s">
-        <v>193</v>
+        <v>264</v>
       </c>
       <c r="E43" t="s">
-        <v>204</v>
+        <v>7</v>
       </c>
       <c r="F43" t="s">
         <v>7</v>
       </c>
       <c r="G43">
-        <v>3.642232244422995E-14</v>
+        <v>5.052178386949745E-32</v>
       </c>
       <c r="H43">
-        <v>0.9878500485823133</v>
+        <v>0.8786754042069094</v>
       </c>
       <c r="I43">
-        <v>0.01054811649070542</v>
+        <v>0.1213240063232884</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -2211,28 +2505,28 @@
         <v>51</v>
       </c>
       <c r="B44" t="s">
-        <v>91</v>
+        <v>118</v>
       </c>
       <c r="C44" t="s">
-        <v>142</v>
+        <v>189</v>
       </c>
       <c r="D44" t="s">
-        <v>194</v>
+        <v>265</v>
       </c>
       <c r="E44" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" t="s">
-        <v>7</v>
+        <v>299</v>
       </c>
       <c r="G44">
-        <v>2.167710561119431E-15</v>
+        <v>0.0003283965181042326</v>
       </c>
       <c r="H44">
-        <v>0.6179795456573646</v>
+        <v>0.2553169682826926</v>
       </c>
       <c r="I44">
-        <v>0.3819963119837507</v>
+        <v>0.3198400666876552</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -2240,28 +2534,28 @@
         <v>52</v>
       </c>
       <c r="B45" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="C45" t="s">
-        <v>143</v>
+        <v>190</v>
       </c>
       <c r="D45" t="s">
-        <v>195</v>
+        <v>266</v>
       </c>
       <c r="E45" t="s">
-        <v>204</v>
+        <v>6</v>
       </c>
       <c r="F45" t="s">
-        <v>204</v>
+        <v>6</v>
       </c>
       <c r="G45">
-        <v>8.674949498752693E-20</v>
+        <v>0.9956316026054296</v>
       </c>
       <c r="H45">
-        <v>0.07377675453781582</v>
+        <v>0.0001367254641525548</v>
       </c>
       <c r="I45">
-        <v>0.04688134931609806</v>
+        <v>0.004231671464606669</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -2269,28 +2563,28 @@
         <v>53</v>
       </c>
       <c r="B46" t="s">
-        <v>93</v>
+        <v>120</v>
       </c>
       <c r="C46" t="s">
-        <v>144</v>
+        <v>191</v>
       </c>
       <c r="D46" t="s">
-        <v>196</v>
+        <v>267</v>
       </c>
       <c r="E46" t="s">
         <v>8</v>
       </c>
       <c r="F46" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G46">
-        <v>5.941949993520454E-28</v>
+        <v>8.628149605361031E-32</v>
       </c>
       <c r="H46">
-        <v>0.9999932722734646</v>
+        <v>0.0008862705747057895</v>
       </c>
       <c r="I46">
-        <v>6.727451855986454E-06</v>
+        <v>0.9991137289867783</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -2298,54 +2592,57 @@
         <v>54</v>
       </c>
       <c r="B47" t="s">
-        <v>94</v>
+        <v>121</v>
       </c>
       <c r="C47" t="s">
-        <v>145</v>
+        <v>192</v>
       </c>
       <c r="D47" t="s">
-        <v>197</v>
+        <v>268</v>
       </c>
       <c r="E47" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F47" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G47">
-        <v>6.646823572388134E-17</v>
+        <v>0.8526427117575939</v>
       </c>
       <c r="H47">
-        <v>0.003786371509625725</v>
+        <v>0.1473561083303607</v>
       </c>
       <c r="I47">
-        <v>0.9853433286385432</v>
+        <v>1.174952686339837E-06</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
         <v>55</v>
       </c>
+      <c r="B48" t="s">
+        <v>122</v>
+      </c>
       <c r="C48" t="s">
-        <v>146</v>
+        <v>193</v>
       </c>
       <c r="D48" t="s">
-        <v>198</v>
+        <v>269</v>
       </c>
       <c r="E48" t="s">
-        <v>8</v>
+        <v>299</v>
       </c>
       <c r="F48" t="s">
-        <v>7</v>
+        <v>299</v>
       </c>
       <c r="G48">
-        <v>2.640647366265963E-15</v>
+        <v>3.540906595318375E-17</v>
       </c>
       <c r="H48">
-        <v>0.9885185908286315</v>
+        <v>1.321589422084236E-07</v>
       </c>
       <c r="I48">
-        <v>0.01148133215054355</v>
+        <v>1.709742569018589E-08</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -2353,28 +2650,28 @@
         <v>56</v>
       </c>
       <c r="B49" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="C49" t="s">
-        <v>147</v>
+        <v>194</v>
       </c>
       <c r="D49" t="s">
-        <v>199</v>
+        <v>270</v>
       </c>
       <c r="E49" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F49" t="s">
-        <v>7</v>
+        <v>299</v>
       </c>
       <c r="G49">
-        <v>2.329438700091206E-15</v>
+        <v>1.329812229504797E-10</v>
       </c>
       <c r="H49">
-        <v>0.7698836604775076</v>
+        <v>1.885047707540565E-07</v>
       </c>
       <c r="I49">
-        <v>0.2176864358560851</v>
+        <v>1.336568801330146E-07</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -2382,57 +2679,54 @@
         <v>57</v>
       </c>
       <c r="B50" t="s">
-        <v>96</v>
+        <v>124</v>
       </c>
       <c r="C50" t="s">
-        <v>148</v>
+        <v>195</v>
       </c>
       <c r="D50" t="s">
-        <v>200</v>
+        <v>271</v>
       </c>
       <c r="E50" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F50" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G50">
-        <v>1.26575974801977E-21</v>
+        <v>0.6938518244625501</v>
       </c>
       <c r="H50">
-        <v>0.9999859109394182</v>
+        <v>0.3061481752782833</v>
       </c>
       <c r="I50">
-        <v>1.24226031217907E-05</v>
+        <v>2.591632044900088E-10</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" t="s">
         <v>58</v>
       </c>
-      <c r="B51" t="s">
-        <v>97</v>
-      </c>
       <c r="C51" t="s">
-        <v>149</v>
+        <v>196</v>
       </c>
       <c r="D51" t="s">
-        <v>201</v>
+        <v>272</v>
       </c>
       <c r="E51" t="s">
         <v>7</v>
       </c>
       <c r="F51" t="s">
-        <v>204</v>
+        <v>8</v>
       </c>
       <c r="G51">
-        <v>1.687140955745973E-18</v>
+        <v>5.592533611138704E-08</v>
       </c>
       <c r="H51">
-        <v>4.789620426938918E-06</v>
+        <v>0.4049566858334458</v>
       </c>
       <c r="I51">
-        <v>3.038787394755729E-07</v>
+        <v>0.5941343635363271</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -2440,28 +2734,28 @@
         <v>59</v>
       </c>
       <c r="B52" t="s">
-        <v>98</v>
+        <v>125</v>
       </c>
       <c r="C52" t="s">
-        <v>150</v>
+        <v>197</v>
       </c>
       <c r="D52" t="s">
-        <v>202</v>
+        <v>273</v>
       </c>
       <c r="E52" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F52" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G52">
-        <v>2.654686827320393E-21</v>
+        <v>0.2877797916954706</v>
       </c>
       <c r="H52">
-        <v>0.9999999970475528</v>
+        <v>0.01584248826286157</v>
       </c>
       <c r="I52">
-        <v>4.821613633340239E-10</v>
+        <v>0.6963777173377617</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -2469,28 +2763,712 @@
         <v>60</v>
       </c>
       <c r="B53" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="C53" t="s">
-        <v>151</v>
+        <v>198</v>
       </c>
       <c r="D53" t="s">
+        <v>274</v>
+      </c>
+      <c r="E53" t="s">
+        <v>8</v>
+      </c>
+      <c r="F53" t="s">
+        <v>7</v>
+      </c>
+      <c r="G53">
+        <v>5.034294039022298E-06</v>
+      </c>
+      <c r="H53">
+        <v>0.9999949654696224</v>
+      </c>
+      <c r="I53">
+        <v>2.363217110382104E-10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" t="s">
+        <v>61</v>
+      </c>
+      <c r="B54" t="s">
+        <v>127</v>
+      </c>
+      <c r="C54" t="s">
+        <v>199</v>
+      </c>
+      <c r="D54" t="s">
+        <v>275</v>
+      </c>
+      <c r="E54" t="s">
+        <v>6</v>
+      </c>
+      <c r="F54" t="s">
+        <v>299</v>
+      </c>
+      <c r="G54">
+        <v>4.584425307483036E-06</v>
+      </c>
+      <c r="H54">
+        <v>0.0002246043181441146</v>
+      </c>
+      <c r="I54">
+        <v>0.001227089720710863</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" t="s">
+        <v>62</v>
+      </c>
+      <c r="B55" t="s">
+        <v>128</v>
+      </c>
+      <c r="C55" t="s">
+        <v>200</v>
+      </c>
+      <c r="D55" t="s">
+        <v>276</v>
+      </c>
+      <c r="E55" t="s">
+        <v>6</v>
+      </c>
+      <c r="F55" t="s">
+        <v>6</v>
+      </c>
+      <c r="G55">
+        <v>0.9652652624964313</v>
+      </c>
+      <c r="H55">
+        <v>0.03453934296002834</v>
+      </c>
+      <c r="I55">
+        <v>0.0001858069444727234</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" t="s">
+        <v>63</v>
+      </c>
+      <c r="C56" t="s">
+        <v>201</v>
+      </c>
+      <c r="D56" t="s">
+        <v>277</v>
+      </c>
+      <c r="E56" t="s">
+        <v>6</v>
+      </c>
+      <c r="F56" t="s">
+        <v>7</v>
+      </c>
+      <c r="G56">
+        <v>0.08340069055799222</v>
+      </c>
+      <c r="H56">
+        <v>0.9165947410207205</v>
+      </c>
+      <c r="I56">
+        <v>4.567782337152108E-06</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" t="s">
+        <v>64</v>
+      </c>
+      <c r="B57" t="s">
+        <v>129</v>
+      </c>
+      <c r="C57" t="s">
+        <v>202</v>
+      </c>
+      <c r="D57" t="s">
+        <v>278</v>
+      </c>
+      <c r="E57" t="s">
+        <v>8</v>
+      </c>
+      <c r="F57" t="s">
+        <v>7</v>
+      </c>
+      <c r="G57">
+        <v>7.430378084535726E-07</v>
+      </c>
+      <c r="H57">
+        <v>0.7919416195372168</v>
+      </c>
+      <c r="I57">
+        <v>0.2074461849218341</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" t="s">
+        <v>65</v>
+      </c>
+      <c r="B58" t="s">
+        <v>130</v>
+      </c>
+      <c r="C58" t="s">
         <v>203</v>
       </c>
-      <c r="E53" t="s">
+      <c r="D58" t="s">
+        <v>279</v>
+      </c>
+      <c r="E58" t="s">
+        <v>6</v>
+      </c>
+      <c r="F58" t="s">
+        <v>7</v>
+      </c>
+      <c r="G58">
+        <v>1.679713619367298E-10</v>
+      </c>
+      <c r="H58">
+        <v>0.7639407226619908</v>
+      </c>
+      <c r="I58">
+        <v>0.2359223477589659</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" t="s">
+        <v>66</v>
+      </c>
+      <c r="C59" t="s">
         <v>204</v>
       </c>
-      <c r="F53" t="s">
-        <v>7</v>
-      </c>
-      <c r="G53">
-        <v>1.142310649424745E-12</v>
-      </c>
-      <c r="H53">
-        <v>0.7432889050677567</v>
-      </c>
-      <c r="I53">
-        <v>0.1576376921222216</v>
+      <c r="D59" t="s">
+        <v>280</v>
+      </c>
+      <c r="E59" t="s">
+        <v>8</v>
+      </c>
+      <c r="F59" t="s">
+        <v>7</v>
+      </c>
+      <c r="G59">
+        <v>0.000379722186688426</v>
+      </c>
+      <c r="H59">
+        <v>0.9982807563378083</v>
+      </c>
+      <c r="I59">
+        <v>0.00133908939112665</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" t="s">
+        <v>67</v>
+      </c>
+      <c r="C60" t="s">
+        <v>205</v>
+      </c>
+      <c r="D60" t="s">
+        <v>281</v>
+      </c>
+      <c r="E60" t="s">
+        <v>6</v>
+      </c>
+      <c r="F60" t="s">
+        <v>6</v>
+      </c>
+      <c r="G60">
+        <v>0.9988472929632045</v>
+      </c>
+      <c r="H60">
+        <v>5.864434238021441E-05</v>
+      </c>
+      <c r="I60">
+        <v>4.5974454304399E-06</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" t="s">
+        <v>68</v>
+      </c>
+      <c r="B61" t="s">
+        <v>131</v>
+      </c>
+      <c r="C61" t="s">
+        <v>206</v>
+      </c>
+      <c r="D61" t="s">
+        <v>282</v>
+      </c>
+      <c r="E61" t="s">
+        <v>6</v>
+      </c>
+      <c r="F61" t="s">
+        <v>299</v>
+      </c>
+      <c r="G61">
+        <v>0.2386538561828027</v>
+      </c>
+      <c r="H61">
+        <v>0.02898214428748684</v>
+      </c>
+      <c r="I61">
+        <v>0.04833149090076882</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" t="s">
+        <v>69</v>
+      </c>
+      <c r="C62" t="s">
+        <v>207</v>
+      </c>
+      <c r="D62" t="s">
+        <v>283</v>
+      </c>
+      <c r="E62" t="s">
+        <v>6</v>
+      </c>
+      <c r="F62" t="s">
+        <v>8</v>
+      </c>
+      <c r="G62">
+        <v>1.373961490329534E-17</v>
+      </c>
+      <c r="H62">
+        <v>0.001211477026033743</v>
+      </c>
+      <c r="I62">
+        <v>0.9987885198430427</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" t="s">
+        <v>70</v>
+      </c>
+      <c r="B63" t="s">
+        <v>132</v>
+      </c>
+      <c r="C63" t="s">
+        <v>208</v>
+      </c>
+      <c r="D63" t="s">
+        <v>284</v>
+      </c>
+      <c r="E63" t="s">
+        <v>8</v>
+      </c>
+      <c r="F63" t="s">
+        <v>8</v>
+      </c>
+      <c r="G63">
+        <v>1.401937030707565E-16</v>
+      </c>
+      <c r="H63">
+        <v>0.001410076201316221</v>
+      </c>
+      <c r="I63">
+        <v>0.6900930778814737</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" t="s">
+        <v>71</v>
+      </c>
+      <c r="B64" t="s">
+        <v>133</v>
+      </c>
+      <c r="C64" t="s">
+        <v>209</v>
+      </c>
+      <c r="D64" t="s">
+        <v>285</v>
+      </c>
+      <c r="E64" t="s">
+        <v>7</v>
+      </c>
+      <c r="F64" t="s">
+        <v>7</v>
+      </c>
+      <c r="G64">
+        <v>0.02286139073444589</v>
+      </c>
+      <c r="H64">
+        <v>0.9749413555461153</v>
+      </c>
+      <c r="I64">
+        <v>0.002197253719241967</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" t="s">
+        <v>72</v>
+      </c>
+      <c r="B65" t="s">
+        <v>134</v>
+      </c>
+      <c r="C65" t="s">
+        <v>210</v>
+      </c>
+      <c r="D65" t="s">
+        <v>286</v>
+      </c>
+      <c r="E65" t="s">
+        <v>6</v>
+      </c>
+      <c r="F65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G65">
+        <v>0.001497870257802577</v>
+      </c>
+      <c r="H65">
+        <v>0.9984391364651952</v>
+      </c>
+      <c r="I65">
+        <v>5.841216744531891E-05</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" t="s">
+        <v>73</v>
+      </c>
+      <c r="B66" t="s">
+        <v>135</v>
+      </c>
+      <c r="C66" t="s">
+        <v>211</v>
+      </c>
+      <c r="D66" t="s">
+        <v>287</v>
+      </c>
+      <c r="E66" t="s">
+        <v>7</v>
+      </c>
+      <c r="F66" t="s">
+        <v>7</v>
+      </c>
+      <c r="G66">
+        <v>3.884012925394493E-05</v>
+      </c>
+      <c r="H66">
+        <v>0.9999531111946762</v>
+      </c>
+      <c r="I66">
+        <v>8.0452491238218E-06</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" t="s">
+        <v>74</v>
+      </c>
+      <c r="B67" t="s">
+        <v>136</v>
+      </c>
+      <c r="C67" t="s">
+        <v>212</v>
+      </c>
+      <c r="D67" t="s">
+        <v>288</v>
+      </c>
+      <c r="E67" t="s">
+        <v>6</v>
+      </c>
+      <c r="F67" t="s">
+        <v>299</v>
+      </c>
+      <c r="G67">
+        <v>6.308087489247247E-10</v>
+      </c>
+      <c r="H67">
+        <v>0.1312743233762676</v>
+      </c>
+      <c r="I67">
+        <v>4.545502077648785E-05</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" t="s">
+        <v>75</v>
+      </c>
+      <c r="B68" t="s">
+        <v>137</v>
+      </c>
+      <c r="C68" t="s">
+        <v>213</v>
+      </c>
+      <c r="D68" t="s">
+        <v>289</v>
+      </c>
+      <c r="E68" t="s">
+        <v>299</v>
+      </c>
+      <c r="F68" t="s">
+        <v>8</v>
+      </c>
+      <c r="G68">
+        <v>2.177114514500721E-08</v>
+      </c>
+      <c r="H68">
+        <v>0.30148516343153</v>
+      </c>
+      <c r="I68">
+        <v>0.5659897755395153</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69" t="s">
+        <v>76</v>
+      </c>
+      <c r="B69" t="s">
+        <v>138</v>
+      </c>
+      <c r="C69" t="s">
+        <v>214</v>
+      </c>
+      <c r="D69" t="s">
+        <v>290</v>
+      </c>
+      <c r="E69" t="s">
+        <v>6</v>
+      </c>
+      <c r="F69" t="s">
+        <v>299</v>
+      </c>
+      <c r="G69">
+        <v>4.702370983736361E-09</v>
+      </c>
+      <c r="H69">
+        <v>4.774758917460246E-05</v>
+      </c>
+      <c r="I69">
+        <v>0.04948677705863726</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" t="s">
+        <v>77</v>
+      </c>
+      <c r="B70" t="s">
+        <v>139</v>
+      </c>
+      <c r="C70" t="s">
+        <v>215</v>
+      </c>
+      <c r="D70" t="s">
+        <v>291</v>
+      </c>
+      <c r="E70" t="s">
+        <v>7</v>
+      </c>
+      <c r="F70" t="s">
+        <v>299</v>
+      </c>
+      <c r="G70">
+        <v>7.627191268982875E-14</v>
+      </c>
+      <c r="H70">
+        <v>4.480082213364123E-09</v>
+      </c>
+      <c r="I70">
+        <v>4.302125444579367E-06</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" t="s">
+        <v>78</v>
+      </c>
+      <c r="B71" t="s">
+        <v>140</v>
+      </c>
+      <c r="C71" t="s">
+        <v>216</v>
+      </c>
+      <c r="D71" t="s">
+        <v>292</v>
+      </c>
+      <c r="E71" t="s">
+        <v>7</v>
+      </c>
+      <c r="F71" t="s">
+        <v>7</v>
+      </c>
+      <c r="G71">
+        <v>0.001306557172167118</v>
+      </c>
+      <c r="H71">
+        <v>0.9986934422312708</v>
+      </c>
+      <c r="I71">
+        <v>5.965001334781574E-10</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" t="s">
+        <v>79</v>
+      </c>
+      <c r="B72" t="s">
+        <v>141</v>
+      </c>
+      <c r="C72" t="s">
+        <v>217</v>
+      </c>
+      <c r="D72" t="s">
+        <v>293</v>
+      </c>
+      <c r="E72" t="s">
+        <v>299</v>
+      </c>
+      <c r="F72" t="s">
+        <v>299</v>
+      </c>
+      <c r="G72">
+        <v>1.343528291703426E-20</v>
+      </c>
+      <c r="H72">
+        <v>0.06506166435654102</v>
+      </c>
+      <c r="I72">
+        <v>0.0001226451014258382</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73" t="s">
+        <v>80</v>
+      </c>
+      <c r="B73" t="s">
+        <v>142</v>
+      </c>
+      <c r="C73" t="s">
+        <v>218</v>
+      </c>
+      <c r="D73" t="s">
+        <v>294</v>
+      </c>
+      <c r="E73" t="s">
+        <v>6</v>
+      </c>
+      <c r="F73" t="s">
+        <v>7</v>
+      </c>
+      <c r="G73">
+        <v>5.06084061827756E-10</v>
+      </c>
+      <c r="H73">
+        <v>0.9954267855843726</v>
+      </c>
+      <c r="I73">
+        <v>0.004572248717500438</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74" t="s">
+        <v>81</v>
+      </c>
+      <c r="B74" t="s">
+        <v>143</v>
+      </c>
+      <c r="C74" t="s">
+        <v>219</v>
+      </c>
+      <c r="D74" t="s">
+        <v>295</v>
+      </c>
+      <c r="E74" t="s">
+        <v>299</v>
+      </c>
+      <c r="F74" t="s">
+        <v>8</v>
+      </c>
+      <c r="G74">
+        <v>0.1092834940608967</v>
+      </c>
+      <c r="H74">
+        <v>0.2457465649131773</v>
+      </c>
+      <c r="I74">
+        <v>0.6446907846481639</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75" t="s">
+        <v>82</v>
+      </c>
+      <c r="B75" t="s">
+        <v>144</v>
+      </c>
+      <c r="C75" t="s">
+        <v>220</v>
+      </c>
+      <c r="D75" t="s">
+        <v>296</v>
+      </c>
+      <c r="E75" t="s">
+        <v>6</v>
+      </c>
+      <c r="F75" t="s">
+        <v>7</v>
+      </c>
+      <c r="G75">
+        <v>0.2151650671973483</v>
+      </c>
+      <c r="H75">
+        <v>0.7805168612813526</v>
+      </c>
+      <c r="I75">
+        <v>0.004264041540446019</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76" t="s">
+        <v>83</v>
+      </c>
+      <c r="B76" t="s">
+        <v>145</v>
+      </c>
+      <c r="C76" t="s">
+        <v>221</v>
+      </c>
+      <c r="D76" t="s">
+        <v>297</v>
+      </c>
+      <c r="E76" t="s">
+        <v>6</v>
+      </c>
+      <c r="F76" t="s">
+        <v>7</v>
+      </c>
+      <c r="G76">
+        <v>0.002365012235471213</v>
+      </c>
+      <c r="H76">
+        <v>0.9976270319053618</v>
+      </c>
+      <c r="I76">
+        <v>7.955859129676371E-06</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77" t="s">
+        <v>84</v>
+      </c>
+      <c r="B77" t="s">
+        <v>146</v>
+      </c>
+      <c r="C77" t="s">
+        <v>222</v>
+      </c>
+      <c r="D77" t="s">
+        <v>298</v>
+      </c>
+      <c r="E77" t="s">
+        <v>8</v>
+      </c>
+      <c r="F77" t="s">
+        <v>299</v>
+      </c>
+      <c r="G77">
+        <v>6.910761314092023E-14</v>
+      </c>
+      <c r="H77">
+        <v>0.3013710776592878</v>
+      </c>
+      <c r="I77">
+        <v>0.09154563458711498</v>
       </c>
     </row>
   </sheetData>

</xml_diff>